<commit_message>
Mise a jour journal d'activité
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SECOND YEAR\Projet Systeme-Escape-Game-Telethon Github\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6F146F-2820-468D-8E05-CC7A6FBB48B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623D0B75-45C3-4B6B-9B28-2D72425E0A70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -261,12 +261,6 @@
     <xf numFmtId="20" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,6 +291,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -620,25 +620,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F159" sqref="F159"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="C160" sqref="C160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="13"/>
+    <col min="1" max="1" width="11.42578125" style="11"/>
     <col min="2" max="2" width="49.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="13"/>
-    <col min="5" max="5" width="43.85546875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="13"/>
+    <col min="4" max="4" width="11.42578125" style="11"/>
+    <col min="5" max="5" width="43.85546875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="20" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="11"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -647,14 +647,14 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="12"/>
+      <c r="G1" s="10"/>
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
@@ -664,7 +664,7 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="89.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2" s="13">
         <v>43844</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -673,20 +673,22 @@
       <c r="C2" s="5">
         <v>0.125</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="17">
         <v>0.125</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="I2" s="21">
+        <v>0.125</v>
+      </c>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="13">
         <v>43845</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -695,34 +697,34 @@
       <c r="C3" s="5">
         <v>0.10416666666666667</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="17">
         <v>0.125</v>
       </c>
-      <c r="G3" s="12"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4" s="13">
         <v>43846</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="12"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="A5" s="13">
         <v>43847</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -731,1077 +733,1077 @@
       <c r="C5" s="5">
         <v>0.20833333333333334</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="12"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="A6" s="13">
         <v>43848</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="12"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="13">
         <v>43849</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="12"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="13">
         <v>43850</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="13">
         <v>43851</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="13">
         <v>43852</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="10"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="13">
         <v>43853</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="12"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="A12" s="13">
         <v>43854</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="12"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="A13" s="13">
         <v>43855</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="12"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+      <c r="A14" s="13">
         <v>43856</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="12"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="10"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="A15" s="13">
         <v>43857</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="12"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="10"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
+      <c r="A16" s="13">
         <v>43858</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="12"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="A17" s="13">
         <v>43859</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="12"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+      <c r="A18" s="13">
         <v>43860</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="12"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="10"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+      <c r="A19" s="13">
         <v>43861</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="12"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="10"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+      <c r="A20" s="13">
         <v>43862</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="12"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="10"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+      <c r="A21" s="13">
         <v>43863</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="12"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="10"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+      <c r="A22" s="13">
         <v>43864</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="12"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+      <c r="A23" s="13">
         <v>43865</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="12"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="10"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="A24" s="13">
         <v>43866</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="12"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="10"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+      <c r="A25" s="13">
         <v>43867</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="12"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="A26" s="13">
         <v>43868</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="12"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
+      <c r="A27" s="13">
         <v>43869</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="12"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="10"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="A28" s="13">
         <v>43870</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="12"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="10"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
+      <c r="A29" s="13">
         <v>43871</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="12"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="10"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
+      <c r="A30" s="13">
         <v>43872</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="12"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="10"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+      <c r="A31" s="13">
         <v>43873</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="12"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="10"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
+      <c r="A32" s="13">
         <v>43874</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="12"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="10"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
+      <c r="A33" s="13">
         <v>43875</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="12"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="10"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+      <c r="A34" s="13">
         <v>43876</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="12"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="10"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
+      <c r="A35" s="13">
         <v>43877</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="12"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
+      <c r="A36" s="13">
         <v>43878</v>
       </c>
       <c r="B36" s="4"/>
-      <c r="E36" s="21"/>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
+      <c r="A37" s="13">
         <v>43879</v>
       </c>
       <c r="B37" s="4"/>
-      <c r="E37" s="21"/>
+      <c r="E37" s="19"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
+      <c r="A38" s="13">
         <v>43880</v>
       </c>
       <c r="B38" s="4"/>
-      <c r="E38" s="21"/>
+      <c r="E38" s="19"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="15">
+      <c r="A39" s="13">
         <v>43881</v>
       </c>
       <c r="B39" s="4"/>
-      <c r="E39" s="21"/>
+      <c r="E39" s="19"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
+      <c r="A40" s="13">
         <v>43882</v>
       </c>
       <c r="B40" s="4"/>
-      <c r="E40" s="21"/>
+      <c r="E40" s="19"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="15">
+      <c r="A41" s="13">
         <v>43883</v>
       </c>
       <c r="B41" s="4"/>
-      <c r="E41" s="21"/>
+      <c r="E41" s="19"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="15">
+      <c r="A42" s="13">
         <v>43884</v>
       </c>
       <c r="B42" s="4"/>
-      <c r="E42" s="21"/>
+      <c r="E42" s="19"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="15">
+      <c r="A43" s="13">
         <v>43885</v>
       </c>
       <c r="B43" s="4"/>
-      <c r="E43" s="21"/>
+      <c r="E43" s="19"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="15">
+      <c r="A44" s="13">
         <v>43886</v>
       </c>
       <c r="B44" s="4"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="15">
+      <c r="A45" s="13">
         <v>43887</v>
       </c>
       <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="15">
+      <c r="A46" s="13">
         <v>43888</v>
       </c>
       <c r="B46" s="4"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="15">
+      <c r="A47" s="13">
         <v>43889</v>
       </c>
       <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="15">
+      <c r="A48" s="13">
         <v>43890</v>
       </c>
       <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="15">
+      <c r="A49" s="13">
         <v>43891</v>
       </c>
       <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="15">
+      <c r="A50" s="13">
         <v>43892</v>
       </c>
       <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="15">
+      <c r="A51" s="13">
         <v>43893</v>
       </c>
       <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="15">
+      <c r="A52" s="13">
         <v>43894</v>
       </c>
       <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="15">
+      <c r="A53" s="13">
         <v>43895</v>
       </c>
       <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="15">
+      <c r="A54" s="13">
         <v>43896</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="15">
+      <c r="A55" s="13">
         <v>43897</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="15">
+      <c r="A56" s="13">
         <v>43898</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="15">
+      <c r="A57" s="13">
         <v>43899</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="15">
+      <c r="A58" s="13">
         <v>43900</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="15">
+      <c r="A59" s="13">
         <v>43901</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="15">
+      <c r="A60" s="13">
         <v>43902</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="15">
+      <c r="A61" s="13">
         <v>43903</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="15">
+      <c r="A62" s="13">
         <v>43904</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="15">
+      <c r="A63" s="13">
         <v>43905</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="15">
+      <c r="A64" s="13">
         <v>43906</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="15">
+      <c r="A65" s="13">
         <v>43907</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="15">
+      <c r="A66" s="13">
         <v>43908</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="15">
+      <c r="A67" s="13">
         <v>43909</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="15">
+      <c r="A68" s="13">
         <v>43910</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="15">
+      <c r="A69" s="13">
         <v>43911</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="15">
+      <c r="A70" s="13">
         <v>43912</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="15">
+      <c r="A71" s="13">
         <v>43913</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="15">
+      <c r="A72" s="13">
         <v>43914</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="15">
+      <c r="A73" s="13">
         <v>43915</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="15">
+      <c r="A74" s="13">
         <v>43916</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="15">
+      <c r="A75" s="13">
         <v>43917</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="15">
+      <c r="A76" s="13">
         <v>43918</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="15">
+      <c r="A77" s="13">
         <v>43919</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="15">
+      <c r="A78" s="13">
         <v>43920</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="15">
+      <c r="A79" s="13">
         <v>43921</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="15">
+      <c r="A80" s="13">
         <v>43922</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="15">
+      <c r="A81" s="13">
         <v>43923</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="15">
+      <c r="A82" s="13">
         <v>43924</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="15">
+      <c r="A83" s="13">
         <v>43925</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="15">
+      <c r="A84" s="13">
         <v>43926</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="15">
+      <c r="A85" s="13">
         <v>43927</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="15">
+      <c r="A86" s="13">
         <v>43928</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="15">
+      <c r="A87" s="13">
         <v>43929</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="15">
+      <c r="A88" s="13">
         <v>43930</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="15">
+      <c r="A89" s="13">
         <v>43931</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="15">
+      <c r="A90" s="13">
         <v>43932</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="15">
+      <c r="A91" s="13">
         <v>43933</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="15">
+      <c r="A92" s="13">
         <v>43934</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="15">
+      <c r="A93" s="13">
         <v>43935</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="15">
+      <c r="A94" s="13">
         <v>43936</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="15">
+      <c r="A95" s="13">
         <v>43937</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="15">
+      <c r="A96" s="13">
         <v>43938</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="15">
+      <c r="A97" s="13">
         <v>43939</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="15">
+      <c r="A98" s="13">
         <v>43940</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="15">
+      <c r="A99" s="13">
         <v>43941</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="15">
+      <c r="A100" s="13">
         <v>43942</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="15">
+      <c r="A101" s="13">
         <v>43943</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="15">
+      <c r="A102" s="13">
         <v>43944</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="15">
+      <c r="A103" s="13">
         <v>43945</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="15">
+      <c r="A104" s="13">
         <v>43946</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="15">
+      <c r="A105" s="13">
         <v>43947</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="15">
+      <c r="A106" s="13">
         <v>43948</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="15">
+      <c r="A107" s="13">
         <v>43949</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="15">
+      <c r="A108" s="13">
         <v>43950</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="15">
+      <c r="A109" s="13">
         <v>43951</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="15">
+      <c r="A110" s="13">
         <v>43952</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="15">
+      <c r="A111" s="13">
         <v>43953</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="15">
+      <c r="A112" s="13">
         <v>43954</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="15">
+      <c r="A113" s="13">
         <v>43955</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="15">
+      <c r="A114" s="13">
         <v>43956</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="15">
+      <c r="A115" s="13">
         <v>43957</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="15">
+      <c r="A116" s="13">
         <v>43958</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="15">
+      <c r="A117" s="13">
         <v>43959</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="15">
+      <c r="A118" s="13">
         <v>43960</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="15">
+      <c r="A119" s="13">
         <v>43961</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="15">
+      <c r="A120" s="13">
         <v>43962</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="15">
+      <c r="A121" s="13">
         <v>43963</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="15">
+      <c r="A122" s="13">
         <v>43964</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="15">
+      <c r="A123" s="13">
         <v>43965</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="15">
+      <c r="A124" s="13">
         <v>43966</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="15">
+      <c r="A125" s="13">
         <v>43967</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="15">
+      <c r="A126" s="13">
         <v>43968</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="15">
+      <c r="A127" s="13">
         <v>43969</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="15">
+      <c r="A128" s="13">
         <v>43970</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="15">
+      <c r="A129" s="13">
         <v>43971</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="15">
+      <c r="A130" s="13">
         <v>43972</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="15">
+      <c r="A131" s="13">
         <v>43973</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="15">
+      <c r="A132" s="13">
         <v>43974</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="15">
+      <c r="A133" s="13">
         <v>43975</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="15">
+      <c r="A134" s="13">
         <v>43976</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="15">
+      <c r="A135" s="13">
         <v>43977</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="15">
+      <c r="A136" s="13">
         <v>43978</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="15">
+      <c r="A137" s="13">
         <v>43979</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="15">
+      <c r="A138" s="13">
         <v>43980</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="15">
+      <c r="A139" s="13">
         <v>43981</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="15">
+      <c r="A140" s="13">
         <v>43982</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="15">
+      <c r="A141" s="13">
         <v>43983</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="15">
+      <c r="A142" s="13">
         <v>43984</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="15">
+      <c r="A143" s="13">
         <v>43985</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="15">
+      <c r="A144" s="13">
         <v>43986</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A145" s="15">
+      <c r="A145" s="13">
         <v>43987</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A146" s="15">
+      <c r="A146" s="13">
         <v>43988</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A147" s="15">
+      <c r="A147" s="13">
         <v>43989</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" s="15">
+      <c r="A148" s="13">
         <v>43990</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="15">
+      <c r="A149" s="13">
         <v>43991</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A150" s="15">
+      <c r="A150" s="13">
         <v>43992</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A151" s="15">
+      <c r="A151" s="13">
         <v>43993</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="15">
+      <c r="A152" s="13">
         <v>43994</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A153" s="15">
+      <c r="A153" s="13">
         <v>43995</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A154" s="15">
+      <c r="A154" s="13">
         <v>43996</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A155" s="15">
+      <c r="A155" s="13">
         <v>43997</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="16" t="s">
+      <c r="A159" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C159" s="9">
         <f>SUM(C2:C155)</f>
         <v>0.4375</v>
       </c>
-      <c r="F159" s="10">
+      <c r="F159" s="9">
         <f>SUM(F2:F155)</f>
         <v>0.25</v>
       </c>
-      <c r="I159" s="11">
+      <c r="I159" s="22">
         <f>SUM(I2:I155)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mise a jour journal d'activités
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SECOND YEAR\Projet Systeme-Escape-Game-Telethon Github\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623D0B75-45C3-4B6B-9B28-2D72425E0A70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B86C238-04E0-4DB9-9E64-175CDB4F1595}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -51,13 +51,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Début des projets : Relecture du dossier de présentation, Création d'un Github ; Utilisation de GitKraken ; Prise de documentation sur l'installation de la Raspberry, de Raspbian et des lecteur de carte RFID</t>
-  </si>
-  <si>
     <t>Création du word pour la revue de projet n°1 et début de ça rédaction (perte du travail, mauvaise utilisation du Git) ; Choix d'un IDE, choix de Pycharm.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création d'un journal d'activité commun </t>
   </si>
   <si>
     <t>Total heures</t>
@@ -68,12 +62,18 @@
   <si>
     <t>Création d'un dossier d'activité, suite du Gantt, création du schéma réseau avec analyse des besoins.</t>
   </si>
+  <si>
+    <t>Lancement du projet : Relecture du dossier de présentation, Création d'un Github ; Utilisation de GitKraken ; Prise de documentation sur l'installation de la Raspberry, de Raspbian et des lecteur de carte RFID</t>
+  </si>
+  <si>
+    <t>Création d'un journal d'activité commun ; Rédaction du word revue de projet n°1 ; Rédaction du Gantt commun ; Digramme de …</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,14 +106,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -225,16 +217,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,20 +233,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -268,16 +249,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="4" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -286,7 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -299,14 +280,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="60 % - Accent1" xfId="6" builtinId="32"/>
+  <cellStyles count="6">
+    <cellStyle name="60 % - Accent1" xfId="5" builtinId="32"/>
     <cellStyle name="Cellule liée" xfId="3" builtinId="24"/>
     <cellStyle name="Neutre" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Texte explicatif" xfId="4" builtinId="53"/>
     <cellStyle name="Titre 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Total" xfId="5" builtinId="25"/>
+    <cellStyle name="Total" xfId="4" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -620,25 +600,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C160" sqref="C160"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="11"/>
+    <col min="1" max="1" width="11.42578125" style="7"/>
     <col min="2" max="2" width="49.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="11"/>
-    <col min="5" max="5" width="43.85546875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="20" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="11"/>
+    <col min="4" max="4" width="11.42578125" style="7"/>
+    <col min="5" max="5" width="43.85546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="7"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -647,14 +627,14 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
@@ -664,1144 +644,1246 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="89.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="9">
         <v>43844</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0.125</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>43845</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C3" s="3">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="13">
         <v>0.125</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="17">
-        <v>0.125</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="21">
-        <v>0.125</v>
-      </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <v>43845</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="17">
-        <v>0.125</v>
-      </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="9">
         <v>43846</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="10"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
         <v>43847</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="10"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="9">
         <v>43848</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="10"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="9">
         <v>43849</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="10"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="9">
         <v>43850</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="10"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="9">
         <v>43851</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="10"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="9">
         <v>43852</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="9">
         <v>43853</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="10"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="9">
         <v>43854</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="10"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="9">
         <v>43855</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="10"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="9">
         <v>43856</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="10"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="A15" s="9">
         <v>43857</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="10"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="A16" s="9">
         <v>43858</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="10"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17" s="9">
         <v>43859</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="10"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A18" s="9">
         <v>43860</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="10"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
+      <c r="A19" s="9">
         <v>43861</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="10"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="A20" s="9">
         <v>43862</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="10"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
+      <c r="A21" s="9">
         <v>43863</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="10"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="6"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+      <c r="A22" s="9">
         <v>43864</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="10"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+      <c r="A23" s="9">
         <v>43865</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="10"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
+      <c r="A24" s="9">
         <v>43866</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="10"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
+      <c r="A25" s="9">
         <v>43867</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="10"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="6"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
+      <c r="A26" s="9">
         <v>43868</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="10"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="6"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
+      <c r="A27" s="9">
         <v>43869</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="10"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="6"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="13">
+      <c r="A28" s="9">
         <v>43870</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="10"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="6"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
+      <c r="A29" s="9">
         <v>43871</v>
       </c>
-      <c r="B29" s="3"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="10"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="6"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
+      <c r="A30" s="9">
         <v>43872</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="10"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="6"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="13">
+      <c r="A31" s="9">
         <v>43873</v>
       </c>
-      <c r="B31" s="3"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="10"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="6"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="13">
+      <c r="A32" s="9">
         <v>43874</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="10"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="6"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="13">
+      <c r="A33" s="9">
         <v>43875</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="10"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="6"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="13">
+      <c r="A34" s="9">
         <v>43876</v>
       </c>
-      <c r="B34" s="3"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="10"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="6"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="13">
+      <c r="A35" s="9">
         <v>43877</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="10"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="6"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="13">
+      <c r="A36" s="9">
         <v>43878</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="E36" s="19"/>
+      <c r="B36" s="12"/>
+      <c r="E36" s="15"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="13">
+      <c r="A37" s="9">
         <v>43879</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="E37" s="19"/>
+      <c r="B37" s="12"/>
+      <c r="E37" s="15"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="13">
+      <c r="A38" s="9">
         <v>43880</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="E38" s="19"/>
+      <c r="B38" s="12"/>
+      <c r="E38" s="15"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="13">
+      <c r="A39" s="9">
         <v>43881</v>
       </c>
-      <c r="B39" s="4"/>
-      <c r="E39" s="19"/>
+      <c r="B39" s="12"/>
+      <c r="E39" s="15"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="13">
+      <c r="A40" s="9">
         <v>43882</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="E40" s="19"/>
+      <c r="B40" s="12"/>
+      <c r="E40" s="15"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="13">
+      <c r="A41" s="9">
         <v>43883</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="E41" s="19"/>
+      <c r="B41" s="12"/>
+      <c r="E41" s="15"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="13">
+      <c r="A42" s="9">
         <v>43884</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="E42" s="19"/>
+      <c r="B42" s="12"/>
+      <c r="E42" s="15"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="13">
+      <c r="A43" s="9">
         <v>43885</v>
       </c>
-      <c r="B43" s="4"/>
-      <c r="E43" s="19"/>
+      <c r="B43" s="12"/>
+      <c r="E43" s="15"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="13">
+      <c r="A44" s="9">
         <v>43886</v>
       </c>
-      <c r="B44" s="4"/>
+      <c r="B44" s="12"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="13">
+      <c r="A45" s="9">
         <v>43887</v>
       </c>
-      <c r="B45" s="4"/>
+      <c r="B45" s="12"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="13">
+      <c r="A46" s="9">
         <v>43888</v>
       </c>
-      <c r="B46" s="4"/>
+      <c r="B46" s="12"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="13">
+      <c r="A47" s="9">
         <v>43889</v>
       </c>
-      <c r="B47" s="4"/>
+      <c r="B47" s="12"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="13">
+      <c r="A48" s="9">
         <v>43890</v>
       </c>
-      <c r="B48" s="4"/>
+      <c r="B48" s="12"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="13">
+      <c r="A49" s="9">
         <v>43891</v>
       </c>
-      <c r="B49" s="4"/>
+      <c r="B49" s="12"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="13">
+      <c r="A50" s="9">
         <v>43892</v>
       </c>
-      <c r="B50" s="4"/>
+      <c r="B50" s="12"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="13">
+      <c r="A51" s="9">
         <v>43893</v>
       </c>
-      <c r="B51" s="4"/>
+      <c r="B51" s="12"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="13">
+      <c r="A52" s="9">
         <v>43894</v>
       </c>
-      <c r="B52" s="4"/>
+      <c r="B52" s="12"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="13">
+      <c r="A53" s="9">
         <v>43895</v>
       </c>
-      <c r="B53" s="4"/>
+      <c r="B53" s="12"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="13">
+      <c r="A54" s="9">
         <v>43896</v>
       </c>
+      <c r="B54" s="12"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="13">
+      <c r="A55" s="9">
         <v>43897</v>
       </c>
+      <c r="B55" s="12"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="13">
+      <c r="A56" s="9">
         <v>43898</v>
       </c>
+      <c r="B56" s="12"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="13">
+      <c r="A57" s="9">
         <v>43899</v>
       </c>
+      <c r="B57" s="12"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="13">
+      <c r="A58" s="9">
         <v>43900</v>
       </c>
+      <c r="B58" s="12"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="13">
+      <c r="A59" s="9">
         <v>43901</v>
       </c>
+      <c r="B59" s="12"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="13">
+      <c r="A60" s="9">
         <v>43902</v>
       </c>
+      <c r="B60" s="12"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="13">
+      <c r="A61" s="9">
         <v>43903</v>
       </c>
+      <c r="B61" s="12"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="13">
+      <c r="A62" s="9">
         <v>43904</v>
       </c>
+      <c r="B62" s="12"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="13">
+      <c r="A63" s="9">
         <v>43905</v>
       </c>
+      <c r="B63" s="12"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="13">
+      <c r="A64" s="9">
         <v>43906</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="13">
+      <c r="B64" s="12"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="9">
         <v>43907</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="13">
+      <c r="B65" s="12"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="9">
         <v>43908</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="13">
+      <c r="B66" s="12"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
         <v>43909</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="13">
+      <c r="B67" s="12"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="9">
         <v>43910</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="13">
+      <c r="B68" s="12"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="9">
         <v>43911</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="13">
+      <c r="B69" s="12"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="9">
         <v>43912</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="13">
+      <c r="B70" s="12"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="9">
         <v>43913</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="13">
+      <c r="B71" s="12"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="9">
         <v>43914</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="13">
+      <c r="B72" s="12"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="9">
         <v>43915</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="13">
+      <c r="B73" s="12"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="9">
         <v>43916</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="13">
+      <c r="B74" s="12"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="9">
         <v>43917</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="13">
+      <c r="B75" s="12"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="9">
         <v>43918</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="13">
+      <c r="B76" s="12"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="9">
         <v>43919</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="13">
+      <c r="B77" s="12"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="9">
         <v>43920</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="13">
+      <c r="B78" s="12"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="9">
         <v>43921</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="13">
+      <c r="B79" s="12"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="9">
         <v>43922</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="13">
+      <c r="B80" s="12"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="9">
         <v>43923</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="13">
+      <c r="B81" s="12"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="9">
         <v>43924</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="13">
+      <c r="B82" s="12"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="9">
         <v>43925</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="13">
+      <c r="B83" s="12"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="9">
         <v>43926</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="13">
+      <c r="B84" s="12"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="9">
         <v>43927</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="13">
+      <c r="B85" s="12"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="9">
         <v>43928</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="13">
+      <c r="B86" s="12"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="9">
         <v>43929</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="13">
+      <c r="B87" s="12"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="9">
         <v>43930</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="13">
+      <c r="B88" s="12"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="9">
         <v>43931</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="13">
+      <c r="B89" s="12"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="9">
         <v>43932</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="13">
+      <c r="B90" s="12"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="9">
         <v>43933</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="13">
+      <c r="B91" s="12"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="9">
         <v>43934</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="13">
+      <c r="B92" s="12"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="9">
         <v>43935</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="13">
+      <c r="B93" s="12"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="9">
         <v>43936</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="13">
+      <c r="B94" s="12"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="9">
         <v>43937</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="13">
+      <c r="B95" s="12"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="9">
         <v>43938</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="13">
+      <c r="B96" s="12"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="9">
         <v>43939</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="13">
+      <c r="B97" s="12"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="9">
         <v>43940</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="13">
+      <c r="B98" s="12"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="9">
         <v>43941</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="13">
+      <c r="B99" s="12"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="9">
         <v>43942</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="13">
+      <c r="B100" s="12"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="9">
         <v>43943</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="13">
+      <c r="B101" s="12"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="9">
         <v>43944</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="13">
+      <c r="B102" s="12"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="9">
         <v>43945</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="13">
+      <c r="B103" s="12"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="9">
         <v>43946</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="13">
+      <c r="B104" s="12"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="9">
         <v>43947</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="13">
+      <c r="B105" s="12"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="9">
         <v>43948</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="13">
+      <c r="B106" s="12"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="9">
         <v>43949</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="13">
+      <c r="B107" s="12"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="9">
         <v>43950</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="13">
+      <c r="B108" s="12"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="9">
         <v>43951</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="13">
+      <c r="B109" s="12"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="9">
         <v>43952</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="13">
+      <c r="B110" s="12"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="9">
         <v>43953</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="13">
+      <c r="B111" s="12"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="9">
         <v>43954</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="13">
+      <c r="B112" s="12"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="9">
         <v>43955</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="13">
+      <c r="B113" s="12"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="9">
         <v>43956</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="13">
+      <c r="B114" s="12"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="9">
         <v>43957</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="13">
+      <c r="B115" s="12"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="9">
         <v>43958</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="13">
+      <c r="B116" s="12"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="9">
         <v>43959</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="13">
+      <c r="B117" s="12"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="9">
         <v>43960</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="13">
+      <c r="B118" s="12"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="9">
         <v>43961</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="13">
+      <c r="B119" s="12"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="9">
         <v>43962</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="13">
+      <c r="B120" s="12"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="9">
         <v>43963</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="13">
+      <c r="B121" s="12"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="9">
         <v>43964</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="13">
+      <c r="B122" s="12"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="9">
         <v>43965</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="13">
+      <c r="B123" s="12"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="9">
         <v>43966</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="13">
+      <c r="B124" s="12"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="9">
         <v>43967</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="13">
+      <c r="B125" s="12"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="9">
         <v>43968</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="13">
+      <c r="B126" s="12"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="9">
         <v>43969</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="13">
+      <c r="B127" s="12"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="9">
         <v>43970</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="13">
+      <c r="B128" s="12"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="9">
         <v>43971</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="13">
+      <c r="B129" s="12"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="9">
         <v>43972</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="13">
+      <c r="B130" s="12"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="9">
         <v>43973</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="13">
+      <c r="B131" s="12"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="9">
         <v>43974</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="13">
+      <c r="B132" s="12"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="9">
         <v>43975</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="13">
+      <c r="B133" s="12"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="9">
         <v>43976</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="13">
+      <c r="B134" s="12"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="9">
         <v>43977</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="13">
+      <c r="B135" s="12"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="9">
         <v>43978</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="13">
+      <c r="B136" s="12"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="9">
         <v>43979</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="13">
+      <c r="B137" s="12"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="9">
         <v>43980</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="13">
+      <c r="B138" s="12"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="9">
         <v>43981</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="13">
+      <c r="B139" s="12"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="9">
         <v>43982</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="13">
+      <c r="B140" s="12"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="9">
         <v>43983</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="13">
+      <c r="B141" s="12"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="9">
         <v>43984</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="13">
+      <c r="B142" s="12"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="9">
         <v>43985</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="13">
+      <c r="B143" s="12"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="9">
         <v>43986</v>
       </c>
+      <c r="B144" s="12"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A145" s="13">
+      <c r="A145" s="9">
         <v>43987</v>
       </c>
+      <c r="B145" s="12"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A146" s="13">
+      <c r="A146" s="9">
         <v>43988</v>
       </c>
+      <c r="B146" s="12"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A147" s="13">
+      <c r="A147" s="9">
         <v>43989</v>
       </c>
+      <c r="B147" s="12"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" s="13">
+      <c r="A148" s="9">
         <v>43990</v>
       </c>
+      <c r="B148" s="12"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="13">
+      <c r="A149" s="9">
         <v>43991</v>
       </c>
+      <c r="B149" s="12"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A150" s="13">
+      <c r="A150" s="9">
         <v>43992</v>
       </c>
+      <c r="B150" s="12"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A151" s="13">
+      <c r="A151" s="9">
         <v>43993</v>
       </c>
+      <c r="B151" s="12"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="13">
+      <c r="A152" s="9">
         <v>43994</v>
       </c>
+      <c r="B152" s="12"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A153" s="13">
+      <c r="A153" s="9">
         <v>43995</v>
       </c>
+      <c r="B153" s="12"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A154" s="13">
+      <c r="A154" s="9">
         <v>43996</v>
       </c>
+      <c r="B154" s="12"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A155" s="13">
+      <c r="A155" s="9">
         <v>43997</v>
       </c>
+      <c r="B155" s="12"/>
     </row>
     <row r="159" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C159" s="9">
+      <c r="A159" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C159" s="5">
         <f>SUM(C2:C155)</f>
         <v>0.4375</v>
       </c>
-      <c r="F159" s="9">
+      <c r="F159" s="5">
         <f>SUM(F2:F155)</f>
         <v>0.25</v>
       </c>
-      <c r="I159" s="22">
+      <c r="I159" s="18">
         <f>SUM(I2:I155)</f>
         <v>0.125</v>
       </c>

</xml_diff>

<commit_message>
MAJ du journal d'activités
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SECOND YEAR\Projet Systeme-Escape-Game-Telethon Github\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C7F204-1E03-4EDD-8773-E69578DC08CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5976B789-D3CC-4FC1-AA4D-9C5D55F13285}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -70,6 +72,12 @@
   </si>
   <si>
     <t>Création d'un journal d'activité commun ; Rédaction du word revue de projet n°1 ; Rédaction du Gantt commun</t>
+  </si>
+  <si>
+    <t>Redefinition des activités sous forme de compte rendu Word. Rédaction de la planification Gantt commune. Analyse des besoins en UML, début d'un diagramme de séquence.</t>
+  </si>
+  <si>
+    <t>Poursuite du diagramme de séquence propre à l'application de supervision souhaitée.</t>
   </si>
 </sst>
 </file>
@@ -130,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +154,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -200,22 +214,26 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thick">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="4"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -228,12 +246,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -249,16 +264,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -282,6 +291,19 @@
     <xf numFmtId="20" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60 % - Accent1" xfId="5" builtinId="32"/>
@@ -604,1293 +626,1301 @@
   <dimension ref="A1:J160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="7"/>
+    <col min="1" max="1" width="11.42578125" style="6"/>
     <col min="2" max="2" width="49.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="7"/>
-    <col min="5" max="5" width="43.85546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="7"/>
+    <col min="4" max="4" width="11.42578125" style="6"/>
+    <col min="5" max="5" width="43.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="6"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" ht="89.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="J1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>43844</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0.125</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="10">
         <v>0.125</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="17">
+      <c r="I2" s="14">
         <v>0.125</v>
       </c>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>43845</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.10416666666666667</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="12" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="10">
         <v>0.125</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>43846</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>43847</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>0.20833333333333334</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G5" s="5"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>43848</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="6"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>43849</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="6"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>43850</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>43851</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="6"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G9" s="5"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <v>43852</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="6"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="7">
         <v>43853</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="6"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>43854</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="6"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="7">
         <v>43855</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="7">
         <v>43856</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="7">
         <v>43857</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="6"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="5"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="7">
         <v>43858</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="6"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="7">
         <v>43859</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="6"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="7">
         <v>43860</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="6"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="7">
         <v>43861</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="6"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="5"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="A20" s="7">
         <v>43862</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="6"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="5"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="7">
         <v>43863</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="6"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="5"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="7">
         <v>43864</v>
       </c>
-      <c r="B22" s="12"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="6"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="7">
         <v>43865</v>
       </c>
-      <c r="B23" s="12"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="6"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="5"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="A24" s="7">
         <v>43866</v>
       </c>
-      <c r="B24" s="12"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="6"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="5"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="A25" s="7">
         <v>43867</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="6"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="5"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="A26" s="7">
         <v>43868</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="9"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="6"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="5"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="7">
         <v>43869</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="6"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="5"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="A28" s="7">
         <v>43870</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="6"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="5"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="7">
         <v>43871</v>
       </c>
-      <c r="B29" s="12"/>
+      <c r="B29" s="9"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="6"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="5"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="A30" s="7">
         <v>43872</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="9"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="6"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="5"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="A31" s="7">
         <v>43873</v>
       </c>
-      <c r="B31" s="12"/>
+      <c r="B31" s="9"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="6"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="5"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="A32" s="7">
         <v>43874</v>
       </c>
-      <c r="B32" s="12"/>
+      <c r="B32" s="9"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="6"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="5"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="A33" s="7">
         <v>43875</v>
       </c>
-      <c r="B33" s="12"/>
+      <c r="B33" s="9"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="6"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="5"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+      <c r="A34" s="7">
         <v>43876</v>
       </c>
-      <c r="B34" s="12"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="6"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="5"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="A35" s="7">
         <v>43877</v>
       </c>
-      <c r="B35" s="12"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="6"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="5"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+      <c r="A36" s="7">
         <v>43878</v>
       </c>
-      <c r="B36" s="12"/>
-      <c r="E36" s="15"/>
+      <c r="B36" s="9"/>
+      <c r="E36" s="12"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+      <c r="A37" s="7">
         <v>43879</v>
       </c>
-      <c r="B37" s="12"/>
-      <c r="E37" s="15"/>
+      <c r="B37" s="9"/>
+      <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+      <c r="A38" s="7">
         <v>43880</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="E38" s="15"/>
+      <c r="B38" s="9"/>
+      <c r="E38" s="12"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="A39" s="7">
         <v>43881</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="E39" s="15"/>
+      <c r="B39" s="9"/>
+      <c r="E39" s="12"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+      <c r="A40" s="7">
         <v>43882</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="E40" s="15"/>
+      <c r="B40" s="9"/>
+      <c r="E40" s="12"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+      <c r="A41" s="7">
         <v>43883</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="E41" s="15"/>
+      <c r="B41" s="9"/>
+      <c r="E41" s="12"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+      <c r="A42" s="7">
         <v>43884</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="E42" s="15"/>
+      <c r="B42" s="9"/>
+      <c r="E42" s="12"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+      <c r="A43" s="7">
         <v>43885</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="E43" s="15"/>
+      <c r="B43" s="9"/>
+      <c r="E43" s="12"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
+      <c r="A44" s="7">
         <v>43886</v>
       </c>
-      <c r="B44" s="12"/>
+      <c r="B44" s="9"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+      <c r="A45" s="7">
         <v>43887</v>
       </c>
-      <c r="B45" s="12"/>
+      <c r="B45" s="9"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+      <c r="A46" s="7">
         <v>43888</v>
       </c>
-      <c r="B46" s="12"/>
+      <c r="B46" s="9"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
+      <c r="A47" s="7">
         <v>43889</v>
       </c>
-      <c r="B47" s="12"/>
+      <c r="B47" s="9"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="9">
+      <c r="A48" s="7">
         <v>43890</v>
       </c>
-      <c r="B48" s="12"/>
+      <c r="B48" s="9"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+      <c r="A49" s="7">
         <v>43891</v>
       </c>
-      <c r="B49" s="12"/>
+      <c r="B49" s="9"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+      <c r="A50" s="7">
         <v>43892</v>
       </c>
-      <c r="B50" s="12"/>
+      <c r="B50" s="9"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
+      <c r="A51" s="7">
         <v>43893</v>
       </c>
-      <c r="B51" s="12"/>
+      <c r="B51" s="9"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+      <c r="A52" s="7">
         <v>43894</v>
       </c>
-      <c r="B52" s="12"/>
+      <c r="B52" s="9"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="9">
+      <c r="A53" s="7">
         <v>43895</v>
       </c>
-      <c r="B53" s="12"/>
+      <c r="B53" s="9"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
+      <c r="A54" s="7">
         <v>43896</v>
       </c>
-      <c r="B54" s="12"/>
+      <c r="B54" s="9"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
+      <c r="A55" s="7">
         <v>43897</v>
       </c>
-      <c r="B55" s="12"/>
+      <c r="B55" s="9"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+      <c r="A56" s="7">
         <v>43898</v>
       </c>
-      <c r="B56" s="12"/>
+      <c r="B56" s="9"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="9">
+      <c r="A57" s="7">
         <v>43899</v>
       </c>
-      <c r="B57" s="12"/>
+      <c r="B57" s="9"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
+      <c r="A58" s="7">
         <v>43900</v>
       </c>
-      <c r="B58" s="12"/>
+      <c r="B58" s="9"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="9">
+      <c r="A59" s="7">
         <v>43901</v>
       </c>
-      <c r="B59" s="12"/>
+      <c r="B59" s="9"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="9">
+      <c r="A60" s="7">
         <v>43902</v>
       </c>
-      <c r="B60" s="12"/>
+      <c r="B60" s="9"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="9">
+      <c r="A61" s="7">
         <v>43903</v>
       </c>
-      <c r="B61" s="12"/>
+      <c r="B61" s="9"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="9">
+      <c r="A62" s="7">
         <v>43904</v>
       </c>
-      <c r="B62" s="12"/>
+      <c r="B62" s="9"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="9">
+      <c r="A63" s="7">
         <v>43905</v>
       </c>
-      <c r="B63" s="12"/>
+      <c r="B63" s="9"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="9">
+      <c r="A64" s="7">
         <v>43906</v>
       </c>
-      <c r="B64" s="12"/>
+      <c r="B64" s="9"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="9">
+      <c r="A65" s="7">
         <v>43907</v>
       </c>
-      <c r="B65" s="12"/>
+      <c r="B65" s="9"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="9">
+      <c r="A66" s="7">
         <v>43908</v>
       </c>
-      <c r="B66" s="12"/>
+      <c r="B66" s="9"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
+      <c r="A67" s="7">
         <v>43909</v>
       </c>
-      <c r="B67" s="12"/>
+      <c r="B67" s="9"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="9">
+      <c r="A68" s="7">
         <v>43910</v>
       </c>
-      <c r="B68" s="12"/>
+      <c r="B68" s="9"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
+      <c r="A69" s="7">
         <v>43911</v>
       </c>
-      <c r="B69" s="12"/>
+      <c r="B69" s="9"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="9">
+      <c r="A70" s="7">
         <v>43912</v>
       </c>
-      <c r="B70" s="12"/>
+      <c r="B70" s="9"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="9">
+      <c r="A71" s="7">
         <v>43913</v>
       </c>
-      <c r="B71" s="12"/>
+      <c r="B71" s="9"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="9">
+      <c r="A72" s="7">
         <v>43914</v>
       </c>
-      <c r="B72" s="12"/>
+      <c r="B72" s="9"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="9">
+      <c r="A73" s="7">
         <v>43915</v>
       </c>
-      <c r="B73" s="12"/>
+      <c r="B73" s="9"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="9">
+      <c r="A74" s="7">
         <v>43916</v>
       </c>
-      <c r="B74" s="12"/>
+      <c r="B74" s="9"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="9">
+      <c r="A75" s="7">
         <v>43917</v>
       </c>
-      <c r="B75" s="12"/>
+      <c r="B75" s="9"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
+      <c r="A76" s="7">
         <v>43918</v>
       </c>
-      <c r="B76" s="12"/>
+      <c r="B76" s="9"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="9">
+      <c r="A77" s="7">
         <v>43919</v>
       </c>
-      <c r="B77" s="12"/>
+      <c r="B77" s="9"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="9">
+      <c r="A78" s="7">
         <v>43920</v>
       </c>
-      <c r="B78" s="12"/>
+      <c r="B78" s="9"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="9">
+      <c r="A79" s="7">
         <v>43921</v>
       </c>
-      <c r="B79" s="12"/>
+      <c r="B79" s="9"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="9">
+      <c r="A80" s="7">
         <v>43922</v>
       </c>
-      <c r="B80" s="12"/>
+      <c r="B80" s="9"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="9">
+      <c r="A81" s="7">
         <v>43923</v>
       </c>
-      <c r="B81" s="12"/>
+      <c r="B81" s="9"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="9">
+      <c r="A82" s="7">
         <v>43924</v>
       </c>
-      <c r="B82" s="12"/>
+      <c r="B82" s="9"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="9">
+      <c r="A83" s="7">
         <v>43925</v>
       </c>
-      <c r="B83" s="12"/>
+      <c r="B83" s="9"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="9">
+      <c r="A84" s="7">
         <v>43926</v>
       </c>
-      <c r="B84" s="12"/>
+      <c r="B84" s="9"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="9">
+      <c r="A85" s="7">
         <v>43927</v>
       </c>
-      <c r="B85" s="12"/>
+      <c r="B85" s="9"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="9">
+      <c r="A86" s="7">
         <v>43928</v>
       </c>
-      <c r="B86" s="12"/>
+      <c r="B86" s="9"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="9">
+      <c r="A87" s="7">
         <v>43929</v>
       </c>
-      <c r="B87" s="12"/>
+      <c r="B87" s="9"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="9">
+      <c r="A88" s="7">
         <v>43930</v>
       </c>
-      <c r="B88" s="12"/>
+      <c r="B88" s="9"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="9">
+      <c r="A89" s="7">
         <v>43931</v>
       </c>
-      <c r="B89" s="12"/>
+      <c r="B89" s="9"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="9">
+      <c r="A90" s="7">
         <v>43932</v>
       </c>
-      <c r="B90" s="12"/>
+      <c r="B90" s="9"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="9">
+      <c r="A91" s="7">
         <v>43933</v>
       </c>
-      <c r="B91" s="12"/>
+      <c r="B91" s="9"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="9">
+      <c r="A92" s="7">
         <v>43934</v>
       </c>
-      <c r="B92" s="12"/>
+      <c r="B92" s="9"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="9">
+      <c r="A93" s="7">
         <v>43935</v>
       </c>
-      <c r="B93" s="12"/>
+      <c r="B93" s="9"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="9">
+      <c r="A94" s="7">
         <v>43936</v>
       </c>
-      <c r="B94" s="12"/>
+      <c r="B94" s="9"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="9">
+      <c r="A95" s="7">
         <v>43937</v>
       </c>
-      <c r="B95" s="12"/>
+      <c r="B95" s="9"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="9">
+      <c r="A96" s="7">
         <v>43938</v>
       </c>
-      <c r="B96" s="12"/>
+      <c r="B96" s="9"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="9">
+      <c r="A97" s="7">
         <v>43939</v>
       </c>
-      <c r="B97" s="12"/>
+      <c r="B97" s="9"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="9">
+      <c r="A98" s="7">
         <v>43940</v>
       </c>
-      <c r="B98" s="12"/>
+      <c r="B98" s="9"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="9">
+      <c r="A99" s="7">
         <v>43941</v>
       </c>
-      <c r="B99" s="12"/>
+      <c r="B99" s="9"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="9">
+      <c r="A100" s="7">
         <v>43942</v>
       </c>
-      <c r="B100" s="12"/>
+      <c r="B100" s="9"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="9">
+      <c r="A101" s="7">
         <v>43943</v>
       </c>
-      <c r="B101" s="12"/>
+      <c r="B101" s="9"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="9">
+      <c r="A102" s="7">
         <v>43944</v>
       </c>
-      <c r="B102" s="12"/>
+      <c r="B102" s="9"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="9">
+      <c r="A103" s="7">
         <v>43945</v>
       </c>
-      <c r="B103" s="12"/>
+      <c r="B103" s="9"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="9">
+      <c r="A104" s="7">
         <v>43946</v>
       </c>
-      <c r="B104" s="12"/>
+      <c r="B104" s="9"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="9">
+      <c r="A105" s="7">
         <v>43947</v>
       </c>
-      <c r="B105" s="12"/>
+      <c r="B105" s="9"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="9">
+      <c r="A106" s="7">
         <v>43948</v>
       </c>
-      <c r="B106" s="12"/>
+      <c r="B106" s="9"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="9">
+      <c r="A107" s="7">
         <v>43949</v>
       </c>
-      <c r="B107" s="12"/>
+      <c r="B107" s="9"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="9">
+      <c r="A108" s="7">
         <v>43950</v>
       </c>
-      <c r="B108" s="12"/>
+      <c r="B108" s="9"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="9">
+      <c r="A109" s="7">
         <v>43951</v>
       </c>
-      <c r="B109" s="12"/>
+      <c r="B109" s="9"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="9">
+      <c r="A110" s="7">
         <v>43952</v>
       </c>
-      <c r="B110" s="12"/>
+      <c r="B110" s="9"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="9">
+      <c r="A111" s="7">
         <v>43953</v>
       </c>
-      <c r="B111" s="12"/>
+      <c r="B111" s="9"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="9">
+      <c r="A112" s="7">
         <v>43954</v>
       </c>
-      <c r="B112" s="12"/>
+      <c r="B112" s="9"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="9">
+      <c r="A113" s="7">
         <v>43955</v>
       </c>
-      <c r="B113" s="12"/>
+      <c r="B113" s="9"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="9">
+      <c r="A114" s="7">
         <v>43956</v>
       </c>
-      <c r="B114" s="12"/>
+      <c r="B114" s="9"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="9">
+      <c r="A115" s="7">
         <v>43957</v>
       </c>
-      <c r="B115" s="12"/>
+      <c r="B115" s="9"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="9">
+      <c r="A116" s="7">
         <v>43958</v>
       </c>
-      <c r="B116" s="12"/>
+      <c r="B116" s="9"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="9">
+      <c r="A117" s="7">
         <v>43959</v>
       </c>
-      <c r="B117" s="12"/>
+      <c r="B117" s="9"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="9">
+      <c r="A118" s="7">
         <v>43960</v>
       </c>
-      <c r="B118" s="12"/>
+      <c r="B118" s="9"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="9">
+      <c r="A119" s="7">
         <v>43961</v>
       </c>
-      <c r="B119" s="12"/>
+      <c r="B119" s="9"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="9">
+      <c r="A120" s="7">
         <v>43962</v>
       </c>
-      <c r="B120" s="12"/>
+      <c r="B120" s="9"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="9">
+      <c r="A121" s="7">
         <v>43963</v>
       </c>
-      <c r="B121" s="12"/>
+      <c r="B121" s="9"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="9">
+      <c r="A122" s="7">
         <v>43964</v>
       </c>
-      <c r="B122" s="12"/>
+      <c r="B122" s="9"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="9">
+      <c r="A123" s="7">
         <v>43965</v>
       </c>
-      <c r="B123" s="12"/>
+      <c r="B123" s="9"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="9">
+      <c r="A124" s="7">
         <v>43966</v>
       </c>
-      <c r="B124" s="12"/>
+      <c r="B124" s="9"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="9">
+      <c r="A125" s="7">
         <v>43967</v>
       </c>
-      <c r="B125" s="12"/>
+      <c r="B125" s="9"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="9">
+      <c r="A126" s="7">
         <v>43968</v>
       </c>
-      <c r="B126" s="12"/>
+      <c r="B126" s="9"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="9">
+      <c r="A127" s="7">
         <v>43969</v>
       </c>
-      <c r="B127" s="12"/>
+      <c r="B127" s="9"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="9">
+      <c r="A128" s="7">
         <v>43970</v>
       </c>
-      <c r="B128" s="12"/>
+      <c r="B128" s="9"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="9">
+      <c r="A129" s="7">
         <v>43971</v>
       </c>
-      <c r="B129" s="12"/>
+      <c r="B129" s="9"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="9">
+      <c r="A130" s="7">
         <v>43972</v>
       </c>
-      <c r="B130" s="12"/>
+      <c r="B130" s="9"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="9">
+      <c r="A131" s="7">
         <v>43973</v>
       </c>
-      <c r="B131" s="12"/>
+      <c r="B131" s="9"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="9">
+      <c r="A132" s="7">
         <v>43974</v>
       </c>
-      <c r="B132" s="12"/>
+      <c r="B132" s="9"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="9">
+      <c r="A133" s="7">
         <v>43975</v>
       </c>
-      <c r="B133" s="12"/>
+      <c r="B133" s="9"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="9">
+      <c r="A134" s="7">
         <v>43976</v>
       </c>
-      <c r="B134" s="12"/>
+      <c r="B134" s="9"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="9">
+      <c r="A135" s="7">
         <v>43977</v>
       </c>
-      <c r="B135" s="12"/>
+      <c r="B135" s="9"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="9">
+      <c r="A136" s="7">
         <v>43978</v>
       </c>
-      <c r="B136" s="12"/>
+      <c r="B136" s="9"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="9">
+      <c r="A137" s="7">
         <v>43979</v>
       </c>
-      <c r="B137" s="12"/>
+      <c r="B137" s="9"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="9">
+      <c r="A138" s="7">
         <v>43980</v>
       </c>
-      <c r="B138" s="12"/>
+      <c r="B138" s="9"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="9">
+      <c r="A139" s="7">
         <v>43981</v>
       </c>
-      <c r="B139" s="12"/>
+      <c r="B139" s="9"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="9">
+      <c r="A140" s="7">
         <v>43982</v>
       </c>
-      <c r="B140" s="12"/>
+      <c r="B140" s="9"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="9">
+      <c r="A141" s="7">
         <v>43983</v>
       </c>
-      <c r="B141" s="12"/>
+      <c r="B141" s="9"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="9">
+      <c r="A142" s="7">
         <v>43984</v>
       </c>
-      <c r="B142" s="12"/>
+      <c r="B142" s="9"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="9">
+      <c r="A143" s="7">
         <v>43985</v>
       </c>
-      <c r="B143" s="12"/>
+      <c r="B143" s="9"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="9">
+      <c r="A144" s="7">
         <v>43986</v>
       </c>
-      <c r="B144" s="12"/>
+      <c r="B144" s="9"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A145" s="9">
+      <c r="A145" s="7">
         <v>43987</v>
       </c>
-      <c r="B145" s="12"/>
+      <c r="B145" s="9"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A146" s="9">
+      <c r="A146" s="7">
         <v>43988</v>
       </c>
-      <c r="B146" s="12"/>
+      <c r="B146" s="9"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A147" s="9">
+      <c r="A147" s="7">
         <v>43989</v>
       </c>
-      <c r="B147" s="12"/>
+      <c r="B147" s="9"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" s="9">
+      <c r="A148" s="7">
         <v>43990</v>
       </c>
-      <c r="B148" s="12"/>
+      <c r="B148" s="9"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="9">
+      <c r="A149" s="7">
         <v>43991</v>
       </c>
-      <c r="B149" s="12"/>
+      <c r="B149" s="9"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A150" s="9">
+      <c r="A150" s="7">
         <v>43992</v>
       </c>
-      <c r="B150" s="12"/>
+      <c r="B150" s="9"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A151" s="9">
+      <c r="A151" s="7">
         <v>43993</v>
       </c>
-      <c r="B151" s="12"/>
+      <c r="B151" s="9"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" s="9">
+      <c r="A152" s="7">
         <v>43994</v>
       </c>
-      <c r="B152" s="12"/>
+      <c r="B152" s="9"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A153" s="9">
+      <c r="A153" s="7">
         <v>43995</v>
       </c>
-      <c r="B153" s="12"/>
+      <c r="B153" s="9"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A154" s="9">
+      <c r="A154" s="7">
         <v>43996</v>
       </c>
-      <c r="B154" s="12"/>
+      <c r="B154" s="9"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A155" s="9">
+      <c r="A155" s="7">
         <v>43997</v>
       </c>
-      <c r="B155" s="12"/>
+      <c r="B155" s="9"/>
     </row>
     <row r="159" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="10" t="s">
+      <c r="A159" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C159" s="4">
         <f>SUM(C2:C155)</f>
         <v>0.52083333333333337</v>
       </c>
-      <c r="F159" s="5">
+      <c r="F159" s="4">
         <f>SUM(F2:F155)</f>
-        <v>0.25</v>
-      </c>
-      <c r="I159" s="18">
+        <v>0.54166666666666674</v>
+      </c>
+      <c r="I159" s="15">
         <f>SUM(I2:I155)</f>
         <v>0.125</v>
       </c>

</xml_diff>

<commit_message>
Mise a jour du journal d'activités
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projet Téléthon\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5976B789-D3CC-4FC1-AA4D-9C5D55F13285}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C151F8FB-62F8-4CF9-BC4D-235778DE425D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -78,6 +76,18 @@
   </si>
   <si>
     <t>Poursuite du diagramme de séquence propre à l'application de supervision souhaitée.</t>
+  </si>
+  <si>
+    <t>Lancement du projet : Annalyse du dossier, création du GitHub (GitKraken),  recherche d'information sur Boostrap et Apache. Debut de rédaction de mon document Word de documentation</t>
+  </si>
+  <si>
+    <t>Mise à jour du Gantt et création du diagramme de séquence</t>
+  </si>
+  <si>
+    <t>Recherche d'information sur le developpement sur Arduino et sur le materiel (buzzer, écran LCD). Poursuite de la rédaction de mon fichier word.</t>
+  </si>
+  <si>
+    <t>Rédaction d'un Gantt commun. Rédaction de mon fichier PowerPoint pour l'oral. Poursuite de la rédaction de mon fichier word.</t>
   </si>
 </sst>
 </file>
@@ -246,7 +256,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -284,9 +294,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -626,7 +633,7 @@
   <dimension ref="A1:J160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,35 +645,35 @@
     <col min="5" max="5" width="43.85546875" style="13" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="13" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="6"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="42.5703125" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:10" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="17" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="18"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
@@ -686,13 +693,15 @@
         <v>0.125</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="14">
+      <c r="H2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2">
         <v>0.125</v>
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>43845</v>
       </c>
@@ -710,8 +719,12 @@
         <v>0.125</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="H3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.125</v>
+      </c>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -746,8 +759,12 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="H5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -812,8 +829,12 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="H9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1920,9 +1941,9 @@
         <f>SUM(F2:F155)</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="I159" s="15">
+      <c r="I159" s="14">
         <f>SUM(I2:I155)</f>
-        <v>0.125</v>
+        <v>0.54166666666666674</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Pousuite du Powerpoint pour la revue R1
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SECOND YEAR\Projet Systeme-Escape-Game-Telethon Github\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECCC2FF-0F53-470B-96FA-1F49288B6F3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3813C61C-B8FA-4B83-83C2-F52184BD016E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="990" windowWidth="18900" windowHeight="11055" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -697,23 +697,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:K159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="11"/>
-    <col min="2" max="2" width="1.85546875" style="26" customWidth="1"/>
+    <col min="2" max="2" width="0.5703125" style="26" customWidth="1"/>
     <col min="3" max="3" width="46.85546875" style="11" customWidth="1"/>
     <col min="4" max="4" width="14" style="5" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="0.7109375" style="17" customWidth="1"/>
     <col min="6" max="6" width="43.85546875" style="13" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="2" style="17" customWidth="1"/>
+    <col min="8" max="8" width="0.7109375" style="17" customWidth="1"/>
     <col min="9" max="9" width="39.140625" style="11" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="2.7109375" style="23" customWidth="1"/>
+    <col min="11" max="11" width="1" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
MAJ DIAPO et COMPTE RENDU d'ACTIVITE
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SECOND YEAR\Projet Systeme-Escape-Game-Telethon Github\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15993DE-1376-4DB6-BFAC-8F909A2373B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00E918D-6277-49B0-B9DA-C669FA7D3935}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="2025" windowWidth="18900" windowHeight="11055" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Création du diaporama pour la revue de projet 1 + Rédaction des définition de l'étudiant 1</t>
+  </si>
+  <si>
+    <t>Création du diaporama support pour la revue 1. Pousuite du diagramme de séquences. Poursuite du dossier étudiant.</t>
+  </si>
+  <si>
+    <t>Pousuite du diaporama support pour la revue 1.</t>
   </si>
 </sst>
 </file>
@@ -638,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +849,7 @@
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>43852</v>
       </c>
@@ -854,8 +860,12 @@
         <v>0.125</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="11"/>
+      <c r="E10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.125</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -942,8 +952,12 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="11"/>
+      <c r="E16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1953,7 +1967,7 @@
       </c>
       <c r="F159" s="4">
         <f>SUM(F2:F155)</f>
-        <v>0.54166666666666674</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="I159" s="14">
         <f>SUM(I2:I155)</f>

</xml_diff>

<commit_message>
MAJ du Rapport d'Activité, MAJ du diaporama
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00E918D-6277-49B0-B9DA-C669FA7D3935}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5251AF-18F9-4BCA-85DC-3EF725EF295C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -268,7 +268,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,6 +323,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60 % - Accent1" xfId="5" builtinId="32"/>
@@ -644,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +871,9 @@
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="20">
+        <v>0.125</v>
+      </c>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -960,7 +965,9 @@
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="I16" s="20">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -968,13 +975,19 @@
         <v>43859</v>
       </c>
       <c r="B17" s="9"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="I17" s="20">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1963,15 +1976,15 @@
       </c>
       <c r="C159" s="4">
         <f>SUM(C2:C155)</f>
-        <v>0.8125</v>
+        <v>0.89583333333333337</v>
       </c>
       <c r="F159" s="4">
         <f>SUM(F2:F155)</f>
-        <v>0.83333333333333337</v>
+        <v>0.91666666666666674</v>
       </c>
       <c r="I159" s="14">
         <f>SUM(I2:I155)</f>
-        <v>0.54166666666666674</v>
+        <v>0.91666666666666674</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
MAJ du Journal d'Activités du groupe
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SECOND YEAR\Projet Systeme-Escape-Game-Telethon Github\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A36F384-DE7E-4BA3-A39D-13B16E1DAC8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECDCBB0-73A6-41B4-9B18-3CC919DBA967}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -109,23 +109,6 @@
   </si>
   <si>
     <t>Rédefinition de la première page du diaporama pour la revue1. Création d'un chemin de fer.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Finalisation du diagramme de Gantt, ainsi que de la revue. 1 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Passage à la revue 1</t>
-    </r>
   </si>
   <si>
     <t>Poursuite de l'ébauche, refléxions sur l'application de supervision.</t>
@@ -168,6 +151,26 @@
   <si>
     <t xml:space="preserve">Finalisation du câble sur Fritzing + adaptation du câble pour les LEDs + revue du diagrame de séquence </t>
   </si>
+  <si>
+    <t>Recherche et aide pour la récupération de l'image provenant de la caméra IP pour le code en C#. Poursuite de la configuration de la caméra IP et création d'un compte MyDlink</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Finalisation du diagramme de Gantt, ainsi que de la revue. 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Passage à la revue 1</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -176,7 +179,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +236,15 @@
       <b/>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -726,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,7 +1070,7 @@
         <v>43859</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2">
         <v>8.3333333333333329E-2</v>
@@ -1091,19 +1103,19 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>43861</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2">
         <v>0.125</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="8" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F19" s="9">
         <v>0.125</v>
@@ -1162,14 +1174,14 @@
         <v>43865</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" s="9">
         <v>8.3333333333333329E-2</v>
@@ -1186,14 +1198,14 @@
         <v>43866</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="2">
         <v>0.125</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F24" s="9">
         <v>0.125</v>
@@ -1222,14 +1234,14 @@
         <v>43868</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="2">
         <v>0.2638888888888889</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F26" s="9">
         <v>0.25</v>
@@ -1281,19 +1293,23 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43872</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="2">
         <v>0.16666666666666666</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="10"/>
+      <c r="E30" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="9">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="G30" s="4"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2107,7 +2123,7 @@
       </c>
       <c r="F159" s="19">
         <f>SUM(F2:F155)</f>
-        <v>1.5</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="I159" s="20">
         <f>SUM(I2:I155)</f>

</xml_diff>

<commit_message>
Maj digramme de séquence + journal d'activité + socket client/server
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SECOND YEAR\Projet Systeme-Escape-Game-Telethon Github\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECDCBB0-73A6-41B4-9B18-3CC919DBA967}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8EC3F7-0F9F-4058-A094-C68AAE5784DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -170,6 +170,12 @@
       </rPr>
       <t>Passage à la revue 1</t>
     </r>
+  </si>
+  <si>
+    <t>Diagramme de séquence</t>
+  </si>
+  <si>
+    <t>Diagramme de séquence + recherche pour client/server socket</t>
   </si>
 </sst>
 </file>
@@ -738,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,8 +1325,12 @@
       <c r="A31" s="6">
         <v>43873</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="1"/>
+      <c r="B31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="18">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="8"/>
       <c r="F31" s="10"/>
@@ -1343,12 +1353,16 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43875</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="1"/>
+      <c r="B33" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="18">
+        <v>0.25</v>
+      </c>
       <c r="D33" s="4"/>
       <c r="E33" s="8"/>
       <c r="F33" s="10"/>
@@ -2119,7 +2133,7 @@
       </c>
       <c r="C159" s="19">
         <f>SUM(C2:C155)</f>
-        <v>1.6909722222222223</v>
+        <v>2.0243055555555554</v>
       </c>
       <c r="F159" s="19">
         <f>SUM(F2:F155)</f>

</xml_diff>

<commit_message>
MAJ du Journal d'activités et remise des activités de mercredi suite à suppression accidentelle. Ajout d'agrégation dans mon diagramme de séquence.
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SECOND YEAR\Projet Systeme-Escape-Game-Telethon Github\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8EC3F7-0F9F-4058-A094-C68AAE5784DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5463C7F5-9092-41C0-B75B-548B18EE39CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>Diagramme de séquence + recherche pour client/server socket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remodelage des diagrammes de séquence. Séparation en plusieurs parties plus détaillées.  </t>
+  </si>
+  <si>
+    <t>Poursuite des diagrammes de séquence. Création d'un modèle relationnel pour la base de données. Création d'un diagramme de classes pour l'application de supervision. Renseignement sur fonction "singreton" en C#. Re-définition des besoins en matière de base de données.</t>
   </si>
 </sst>
 </file>
@@ -744,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,9 +1096,7 @@
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="18">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="I17" s="18"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1128,9 +1132,7 @@
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="18">
-        <v>0.25</v>
-      </c>
+      <c r="I19" s="18"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1194,9 +1196,7 @@
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="18">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="I23" s="18"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1321,7 +1321,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>43873</v>
       </c>
@@ -1332,8 +1332,12 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D31" s="4"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="10"/>
+      <c r="E31" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G31" s="4"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1353,7 +1357,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>43875</v>
       </c>
@@ -1364,8 +1368,12 @@
         <v>0.25</v>
       </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="10"/>
+      <c r="E33" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="G33" s="4"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2137,11 +2145,11 @@
       </c>
       <c r="F159" s="19">
         <f>SUM(F2:F155)</f>
-        <v>1.6666666666666667</v>
+        <v>1.9166666666666667</v>
       </c>
       <c r="I159" s="20">
         <f>SUM(I2:I155)</f>
-        <v>1.25</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mise à jour de la revue2. MAJ des diagrammes de séquence. Mise à jour du compte rendu d'activités.
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projet Téléthon\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638B3643-0822-438D-995C-9F2FA2200FC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956B8A90-C992-4570-923C-8C81B91961B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Réflexion général sur mes deux parties</t>
+  </si>
+  <si>
+    <t>Mise à jour du diagramme de Gantt. Poursuite du diaporama de revue 2. Mise à jour des diagrammes de séquence et mise en commun de certaines parties avec Guillaume.</t>
   </si>
 </sst>
 </file>
@@ -788,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,7 +1140,7 @@
         <v>41</v>
       </c>
       <c r="I17" s="17">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J17" s="1"/>
     </row>
@@ -1620,13 +1623,17 @@
       <c r="F50" s="10"/>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>43893</v>
       </c>
       <c r="B51" s="8"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
+      <c r="E51" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2353,11 +2360,11 @@
       </c>
       <c r="F159" s="18">
         <f>SUM(F2:F155)</f>
-        <v>2</v>
+        <v>2.0833333333333335</v>
       </c>
       <c r="I159" s="19">
         <f>SUM(I2:I155)</f>
-        <v>2</v>
+        <v>1.9583333333333333</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Maj diapo revue 2 + Journal d'activité
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SECOND YEAR\Projet Systeme-Escape-Game-Telethon Github\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D15F3B3-1D97-4212-8302-76CDB9E98EBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDD2C46-44D5-4E7E-9503-E38067BA3640}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -115,23 +115,6 @@
   </si>
   <si>
     <t>Recherche bus SPI</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Finalisation de la revue 1. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Passage de la revue 1</t>
-    </r>
   </si>
   <si>
     <t>Travail sur le diapo pour la revue 1</t>
@@ -231,6 +214,40 @@
   </si>
   <si>
     <t>Correction des diagrammes de séquences et ajout de nouvelles fonctions. Poursuite du diaporama de revue 2. Apport dans l'ébauche de l'application de supervision.</t>
+  </si>
+  <si>
+    <r>
+      <t>Finalisation de la revue 1.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Passage de la revue 1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalisation du digramme de squence pour le serveur socket asynchrone + préparation du diapo pour la revue 2 </t>
+  </si>
+  <si>
+    <t>recherche pour client/server socket</t>
   </si>
 </sst>
 </file>
@@ -296,14 +313,13 @@
     <font>
       <b/>
       <i/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <i/>
       <sz val="14"/>
       <color theme="1"/>
@@ -420,7 +436,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -463,6 +479,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -786,7 +805,7 @@
   <dimension ref="A1:I160"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +962,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I9" s="1">
         <v>8.3333333333333329E-2</v>
@@ -966,7 +985,7 @@
         <v>0.125</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I10" s="1">
         <v>0.125</v>
@@ -1024,7 +1043,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I16" s="1">
         <v>0.16666666666666666</v>
@@ -1035,7 +1054,7 @@
         <v>43859</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1">
         <v>4.1666666666666664E-2</v>
@@ -1047,7 +1066,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I17" s="1">
         <v>4.1666666666666664E-2</v>
@@ -1065,13 +1084,13 @@
         <v>43861</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="1">
         <v>0.125</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="6">
         <v>0.125</v>
@@ -1106,7 +1125,7 @@
         <v>43865</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1118,7 +1137,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I23" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1141,7 +1160,7 @@
         <v>0.125</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I24" s="1">
         <v>0.125</v>
@@ -1171,7 +1190,7 @@
         <v>0.25</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I26" s="1">
         <v>0.25</v>
@@ -1203,19 +1222,19 @@
         <v>43872</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F30" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I30" s="1">
         <v>0.16666666666666666</v>
@@ -1226,19 +1245,19 @@
         <v>43873</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F31" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I31" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1256,22 +1275,22 @@
         <v>43875</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="1">
         <v>0.25</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F33" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I33" s="1">
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1355,18 +1374,14 @@
         <v>43887</v>
       </c>
       <c r="B45" s="5"/>
+      <c r="C45" s="1"/>
       <c r="E45" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F45" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="H45" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I45" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
@@ -1386,115 +1401,142 @@
       </c>
       <c r="B48" s="5"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>43891</v>
       </c>
       <c r="B49" s="5"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>43892</v>
       </c>
       <c r="B50" s="5"/>
     </row>
-    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>43893</v>
       </c>
-      <c r="B51" s="5"/>
+      <c r="B51" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="E51" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F51" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="H51" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I51" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>43894</v>
       </c>
-      <c r="B52" s="5"/>
+      <c r="B52" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.125</v>
+      </c>
       <c r="E52" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F52" s="6">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I52" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>43895</v>
       </c>
       <c r="B53" s="5"/>
     </row>
-    <row r="54" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>43896</v>
       </c>
-      <c r="B54" s="5"/>
+      <c r="B54" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.25</v>
+      </c>
       <c r="E54" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F54" s="6">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>43897</v>
       </c>
       <c r="B55" s="5"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>43898</v>
       </c>
       <c r="B56" s="5"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>43899</v>
       </c>
       <c r="B57" s="5"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>43900</v>
       </c>
       <c r="B58" s="5"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>43901</v>
       </c>
       <c r="B59" s="5"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>43902</v>
       </c>
       <c r="B60" s="5"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>43903</v>
       </c>
       <c r="B61" s="5"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>43904</v>
       </c>
       <c r="B62" s="5"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>43905</v>
       </c>
       <c r="B63" s="5"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>43906</v>
       </c>
@@ -2052,15 +2094,15 @@
       </c>
       <c r="C159" s="9">
         <f>SUM(C2:C155)</f>
-        <v>1.9826388888888886</v>
+        <v>2.4409722222222219</v>
       </c>
       <c r="F159" s="9">
         <f>SUM(F2:F155)</f>
-        <v>2.3333333333333335</v>
+        <v>2.4583333333333335</v>
       </c>
       <c r="I159" s="10">
         <f>SUM(I2:I155)</f>
-        <v>1.9583333333333333</v>
+        <v>2.4166666666666665</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Maj journal d'activité + diagramme de classe
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SECOND YEAR\Projet Systeme-Escape-Game-Telethon Github\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E63A9B-46F4-480A-AE80-676079851A4B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF49F7A3-B722-4204-8139-BFFFFC48C68F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t xml:space="preserve">Correction des diagrammes de séquences et ajout de nouvelles fonctions. Poursuite du diaporama de revue 2. Apport dans l'ébauche de l'application de supervision. Modification du diagramme de classes. </t>
+  </si>
+  <si>
+    <t>Diagramme de classe + diapo revue 2</t>
   </si>
 </sst>
 </file>
@@ -810,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,7 +1514,12 @@
       <c r="A58" s="3">
         <v>43900</v>
       </c>
-      <c r="B58" s="5"/>
+      <c r="B58" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0.16666666666666666</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
@@ -2101,7 +2109,7 @@
       </c>
       <c r="C159" s="9">
         <f>SUM(C2:C155)</f>
-        <v>2.4409722222222219</v>
+        <v>2.6076388888888884</v>
       </c>
       <c r="F159" s="9">
         <f>SUM(F2:F155)</f>

</xml_diff>

<commit_message>
Mise à jour du journal d'activités (non réalisé hier).
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SECOND YEAR\Projet Systeme-Escape-Game-Telethon Github\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF49F7A3-B722-4204-8139-BFFFFC48C68F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0622C01F-833E-4C48-84B9-17BE57646038}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>Diagramme de classe + diapo revue 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poursuite du diagramme de classes. Poursuite du diaporama de revue 2. Ajout et modification horaires dans le diagramme de Gantt (achevement des tâches). </t>
   </si>
 </sst>
 </file>
@@ -814,7 +817,7 @@
   <dimension ref="A1:J160"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,7 +1513,7 @@
       </c>
       <c r="B57" s="5"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>43900</v>
       </c>
@@ -1518,6 +1521,15 @@
         <v>55</v>
       </c>
       <c r="C58" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F58" s="6">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I58" s="1">
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -2113,11 +2125,11 @@
       </c>
       <c r="F159" s="9">
         <f>SUM(F2:F155)</f>
-        <v>2.4583333333333335</v>
+        <v>2.625</v>
       </c>
       <c r="I159" s="10">
         <f>SUM(I2:I155)</f>
-        <v>2.4166666666666665</v>
+        <v>2.583333333333333</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mise à jour du journal d'activités.
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.guigand\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0622C01F-833E-4C48-84B9-17BE57646038}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228B4F8F-C26B-49CF-B37D-18E6A2E96505}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t xml:space="preserve">Poursuite du diagramme de classes. Poursuite du diaporama de revue 2. Ajout et modification horaires dans le diagramme de Gantt (achevement des tâches). </t>
+  </si>
+  <si>
+    <t>Poursuite du diagramme de classes (définition des multiplicités et des noms). Ajout de celui-ci dans le diaporama de revue 2. Création d'un chemin de fer dans le diaporama et finalisation / entrainement pour la revue 2.</t>
   </si>
 </sst>
 </file>
@@ -816,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E76" sqref="E72:E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,11 +1536,23 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>43901</v>
       </c>
       <c r="B59" s="5"/>
+      <c r="C59" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F59" s="6">
+        <v>0.125</v>
+      </c>
+      <c r="I59" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
@@ -2121,15 +2136,15 @@
       </c>
       <c r="C159" s="9">
         <f>SUM(C2:C155)</f>
-        <v>2.6076388888888884</v>
+        <v>2.6909722222222219</v>
       </c>
       <c r="F159" s="9">
         <f>SUM(F2:F155)</f>
-        <v>2.625</v>
+        <v>2.75</v>
       </c>
       <c r="I159" s="10">
         <f>SUM(I2:I155)</f>
-        <v>2.583333333333333</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remise à jour du journal d'activités
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Guillaume\BTS SN\Projet Systeme-Escape-Game-Telethon\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93C5E4D-B7D5-4CFC-A0B0-9EFE928E3A79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABD25C6-027F-41AA-9F6A-095B743F637B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t>Reprise du diaporama pour la revue 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalisation de la configuration de Visual Studio. Poursuite de l'application de supervision. Etude approfondie de l'adaptateur RS232 - Wi-Fi (en parallèle avec un travail en ESLA sur ce même adaptateur). </t>
   </si>
 </sst>
 </file>
@@ -887,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E69" sqref="E67:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,102 +1683,106 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>43907</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C65" s="1">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="1"/>
+      <c r="E65" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F65" s="6">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>43908</v>
       </c>
       <c r="B66" s="5"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>43909</v>
       </c>
       <c r="B67" s="5"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>43910</v>
       </c>
       <c r="B68" s="5"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>43911</v>
       </c>
       <c r="B69" s="5"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>43912</v>
       </c>
       <c r="B70" s="5"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>43913</v>
       </c>
       <c r="B71" s="5"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>43914</v>
       </c>
       <c r="B72" s="5"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>43915</v>
       </c>
       <c r="B73" s="5"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>43916</v>
       </c>
       <c r="B74" s="5"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>43917</v>
       </c>
       <c r="B75" s="5"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>43918</v>
       </c>
       <c r="B76" s="5"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>43919</v>
       </c>
       <c r="B77" s="5"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>43920</v>
       </c>
       <c r="B78" s="5"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>43921</v>
       </c>
       <c r="B79" s="5"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>43922</v>
       </c>
@@ -2237,11 +2244,11 @@
       </c>
       <c r="C159" s="9">
         <f>SUM(C2:C155)</f>
-        <v>3.1701388888888888</v>
+        <v>3.0451388888888888</v>
       </c>
       <c r="F159" s="9">
         <f>SUM(F2:F155)</f>
-        <v>3.125</v>
+        <v>3.3125</v>
       </c>
       <c r="I159" s="10">
         <f>SUM(I2:I155)</f>

</xml_diff>

<commit_message>
Ajout du programme Relais + thread + maj journal d'activité
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Guillaume\BTS SN\Projet Systeme-Escape-Game-Telethon\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132B7EED-F7E7-4F4B-A8B0-7C6B0307DE9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D97915E-31A1-4875-AB64-E7CC62F1D462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="134">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -518,6 +518,18 @@
   </si>
   <si>
     <t>Poursuite du rapport de conception et étude de certains élements pour présentation. Apport de quelques corrections sur l'application de supervision avec l'aide en Visio de Monsieur HOURDIN. Changement des paramètres de la fenêtre de confirmation de fin de partie et création d'une fonction "Terminer Partie()" auquel Guillaume pourra déposer la partie Socket Client-Serveur.</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport de conception</t>
+  </si>
+  <si>
+    <t>Ecriture du programme pour le module relais.</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport de conception.</t>
+  </si>
+  <si>
+    <t>Reception des jumpers manquant pour faire correctement les tests. Test du programme pour le module relais (programme tourne correctement mais aucun son de déclanchement entendu). Branchement de deux lecteur RFID et test des deux lecteurs, seul le premier branché fonctionne. Recherche sur les thread en python asynchrone qui permettrait de n'avoir aucune boucle "d'écoute" bloquante.</t>
   </si>
 </sst>
 </file>
@@ -1126,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,7 +2450,12 @@
       <c r="A99" s="3">
         <v>43941</v>
       </c>
-      <c r="B99" s="5"/>
+      <c r="B99" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C99" s="1">
+        <v>0.125</v>
+      </c>
       <c r="E99" s="5" t="s">
         <v>122</v>
       </c>
@@ -2450,7 +2467,12 @@
       <c r="A100" s="3">
         <v>43942</v>
       </c>
-      <c r="B100" s="5"/>
+      <c r="B100" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C100" s="1">
+        <v>0.125</v>
+      </c>
       <c r="E100" s="5" t="s">
         <v>123</v>
       </c>
@@ -2462,7 +2484,12 @@
       <c r="A101" s="3">
         <v>43943</v>
       </c>
-      <c r="B101" s="5"/>
+      <c r="B101" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C101" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="E101" s="5" t="s">
         <v>124</v>
       </c>
@@ -2474,7 +2501,12 @@
       <c r="A102" s="3">
         <v>43944</v>
       </c>
-      <c r="B102" s="5"/>
+      <c r="B102" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C102" s="1">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="E102" s="5" t="s">
         <v>125</v>
       </c>
@@ -2486,7 +2518,12 @@
       <c r="A103" s="3">
         <v>43945</v>
       </c>
-      <c r="B103" s="5"/>
+      <c r="B103" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C103" s="1">
+        <v>0.125</v>
+      </c>
       <c r="E103" s="5" t="s">
         <v>126</v>
       </c>
@@ -2510,7 +2547,12 @@
       <c r="A106" s="3">
         <v>43948</v>
       </c>
-      <c r="B106" s="5"/>
+      <c r="B106" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C106" s="1">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="E106" s="5" t="s">
         <v>127</v>
       </c>
@@ -2522,7 +2564,12 @@
       <c r="A107" s="3">
         <v>43949</v>
       </c>
-      <c r="B107" s="5"/>
+      <c r="B107" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C107" s="1">
+        <v>0.25</v>
+      </c>
       <c r="E107" s="5" t="s">
         <v>128</v>
       </c>
@@ -2534,7 +2581,12 @@
       <c r="A108" s="3">
         <v>43950</v>
       </c>
-      <c r="B108" s="5"/>
+      <c r="B108" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C108" s="1">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="E108" s="5" t="s">
         <v>129</v>
       </c>
@@ -2830,7 +2882,7 @@
       </c>
       <c r="C159" s="9">
         <f>SUM(C2:C155)</f>
-        <v>4.8784722222222214</v>
+        <v>6.2951388888888875</v>
       </c>
       <c r="F159" s="9">
         <f>SUM(F2:F155)</f>

</xml_diff>

<commit_message>
Mise à jour du journal d'activités - Correction de l'orthographe.
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Guillaume\BTS SN\Projet Systeme-Escape-Game-Telethon\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6865D1A7-19D9-40BD-978C-22A6F99FE899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A6933A-FBB2-4181-ADF9-68DCA742D13B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="182">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -53,9 +53,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Création du word pour la revue de projet n°1 et début de ça rédaction (perte du travail, mauvaise utilisation du Git) ; Choix d'un IDE, choix de Pycharm.</t>
-  </si>
-  <si>
     <t>Total heures</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Rédaction du diagramme de séquence</t>
   </si>
   <si>
-    <t>Création d'un journal d'activité commun ; Rédaction du word revue de projet n°1 ; Rédaction du Gantt commun</t>
-  </si>
-  <si>
     <t>Redefinition des activités sous forme de compte rendu Word. Rédaction de la planification Gantt commune. Analyse des besoins en UML, début d'un diagramme de séquence.</t>
   </si>
   <si>
@@ -86,12 +80,6 @@
     <t>Recherche d'information sur le developpement sur Arduino et sur le materiel (buzzer, écran LCD). Poursuite de la rédaction de mon fichier word.</t>
   </si>
   <si>
-    <t>Rédaction des définition de l'étudiant 1</t>
-  </si>
-  <si>
-    <t>Création du diaporama pour la revue de projet 1 + Rédaction des définition de l'étudiant 1</t>
-  </si>
-  <si>
     <t>Création du diaporama support pour la revue 1. Pousuite du diagramme de séquences. Poursuite du dossier étudiant.</t>
   </si>
   <si>
@@ -113,12 +101,6 @@
     <t>Poursuite et modification majeure de l'ébauche. Rencontre d'un problème avec l'upload d'un fichier de plus de 100Mo dans GitHub.</t>
   </si>
   <si>
-    <t>Création d'un "Fritzing" (modèle de cablage) sur une platine d'essaye + apport Gantt</t>
-  </si>
-  <si>
-    <t>Recherche bus SPI</t>
-  </si>
-  <si>
     <t>Travail sur le diapo pour la revue 1</t>
   </si>
   <si>
@@ -126,9 +108,6 @@
   </si>
   <si>
     <t xml:space="preserve">Finalisation du câble sur Fritzing + adaptation du câble pour les LEDs + revue du diagrame de séquence </t>
-  </si>
-  <si>
-    <t>Recherche et aide pour la récupération de l'image provenant de la caméra IP pour le code en C#. Poursuite de la configuration de la caméra IP et création d'un compte MyDlink</t>
   </si>
   <si>
     <r>
@@ -151,13 +130,7 @@
     <t>Diagramme de séquence</t>
   </si>
   <si>
-    <t>Diagramme de séquence + recherche pour client/server socket</t>
-  </si>
-  <si>
     <t xml:space="preserve">Remodelage des diagrammes de séquence. Séparation en plusieurs parties plus détaillées.  </t>
-  </si>
-  <si>
-    <t>Poursuite des diagrammes de séquence. Création d'un modèle relationnel pour la base de données. Création d'un diagramme de classes pour l'application de supervision. Renseignement sur fonction "singreton" en C#. Re-définition des besoins en matière de base de données.</t>
   </si>
   <si>
     <t>Modification de l'ébauche de l'application. Reprise du diaporama de présentation pour la revue 2.</t>
@@ -227,12 +200,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Finalisation du digramme de squence pour le serveur socket asynchrone + préparation du diapo pour la revue 2 </t>
-  </si>
-  <si>
-    <t>recherche pour client/server socket</t>
-  </si>
-  <si>
     <t xml:space="preserve">Correction des diagrammes de séquences et ajout de nouvelles fonctions. Poursuite du diaporama de revue 2. Apport dans l'ébauche de l'application de supervision. Modification du diagramme de classes. </t>
   </si>
   <si>
@@ -245,38 +212,12 @@
     <t>Poursuite du diagramme de classes (définition des multiplicités et des noms). Ajout de celui-ci dans le diaporama de revue 2. Création d'un chemin de fer dans le diaporama et finalisation / entrainement pour la revue 2.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Passage à la revue 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Poursuite du diaporama de revue. Poursuite et reinterprétation des analyses UML. Début de l'installation de DEBIAN (erreur carte SD a formatée en ligne de commandes) -&gt; Debian non installé.</t>
-    </r>
-  </si>
-  <si>
     <t>Diaporama et poursuite de l'UML.</t>
   </si>
   <si>
     <t>Mise à jour et intégration du projet dans la Visual Studio sur mon ordinateur personnel. Tentative de correction des erreures liées aux librairies manquantes.</t>
   </si>
   <si>
-    <t>Installation de raspbian + activation de du bus spi, port GPIO + installation de l'IDE phychram(problème d'installation, non finalisé)</t>
-  </si>
-  <si>
     <t>Reprise du diaporama pour la revue 2</t>
   </si>
   <si>
@@ -316,9 +257,6 @@
     <t>Tentative de résolution de l'erreur</t>
   </si>
   <si>
-    <t xml:space="preserve">Résolutions de l'erreur d'installation (installation pycharm compléter) + installation de jdk </t>
-  </si>
-  <si>
     <t xml:space="preserve">Création des différentes fenêtres de l'application de supervision et liens entre elles. Importation de la charte graphique (icônes et formes) dans celle-ci. Recherches sur la base de données. Création de la base de données avec PHPMyAdmin et MYSQL pour liaison avec l'application. Lecture d'un tutoriel permettant cela. </t>
   </si>
   <si>
@@ -328,12 +266,6 @@
     <t>Tentative de récupération de l'uid</t>
   </si>
   <si>
-    <t>Application de supervision : Etude la connexion avec la base de données (tutoriel) et début de mise en œuvre pour la fenêtre d'envoi d'indice. Résolution d'un problème avec une surcharge de Teams rendant impossible l'utilisation de Visual Studio (30 min).</t>
-  </si>
-  <si>
-    <t>Tentative de récupération de l'uid (bug clavier, rend la navigation difficile) + Installation d'Anydesk pour une prise en main facilité</t>
-  </si>
-  <si>
     <t>Programmation page de modification, d'ajout, de suppression d'un compte superviseur</t>
   </si>
   <si>
@@ -346,24 +278,15 @@
     <t xml:space="preserve">Recontre d'un problème avec l'envoi des données de l'équipe vers la Base de données. Recherches sur forum et résolution avec la fonction de requête "NOW()" de MYSQL. </t>
   </si>
   <si>
-    <t>Tentative de récupération de l'uid (difficulté de récupération des fonction de la library)</t>
-  </si>
-  <si>
     <t>Programmation page superviseur, pour gerer les créneaux (formulaire d'ajout, de suppression, de modification)</t>
   </si>
   <si>
     <t>Programmation page pour reserver un créneau ( calendrier avec les dates disponibles et formulaire de réservation). Ajout d'une table MySQL "events" pour gerer les événements du calendrier</t>
   </si>
   <si>
-    <t xml:space="preserve">Poursuite des tests et approfondissement de la communication entre la base de données et l'application. Extraction du script de la BDD. Recherches et test (implémentation) de code pour l'affichage du chronometre dans la fenêtre principale. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Finalisation et tests du chronometre. Création de la fenêtre de fin de partie et création de la méthode permettant l'ouverture de celle-ci lorsque le temps est écoulé. </t>
   </si>
   <si>
-    <t>Recherches et création d'une requête SQL permettant d'insérer l'heure de fin de partie dans le dernier enregistrement (correspondant à l'équipe en cours). Mise en place dans l'application et test validés. Création d'une méthode de mise à jour du score en fin de partie, non terminée.</t>
-  </si>
-  <si>
     <t>Mise à jour de la bdd, essayer de comprendre les roles et comment cela marche</t>
   </si>
   <si>
@@ -385,21 +308,6 @@
     <t>Création des bases pour les rapports d'analyse et de conception communs. Recherches et tests de plusieurs méthodes avec DATASET pour classer les résultats d'une requête SQL dans un tableau de la fenêtre. Recherches non abouties.</t>
   </si>
   <si>
-    <t>Résolution de problème de lié à la librérie et de son emplacement pour que le programme puisse y avoir accès.</t>
-  </si>
-  <si>
-    <t>Identification du problème des librérires avec la fonction "wait_for_tag" qui pose problème.</t>
-  </si>
-  <si>
-    <t>Programme ne ce lance pas avec le message d'erreur suivant "python: can't open file 'RecupUID.py': [Errno 2] No such file or directory".</t>
-  </si>
-  <si>
-    <t>Programme ne ce lance pas avec même message d'erreur suivant "python: can't open file 'RecupUID.py': [Errno 2] No such file or directory".</t>
-  </si>
-  <si>
-    <t>Recherche dans les différents chemins de fichier pour trouver l'origine du problème lier à l'erreur.</t>
-  </si>
-  <si>
     <t>mise à jour bdd, programmation sur l'application Arduino</t>
   </si>
   <si>
@@ -413,9 +321,6 @@
   </si>
   <si>
     <t>test d'un remplacement du "self" part "rdr" dans la fonction wait_for_tag. Sans changement.</t>
-  </si>
-  <si>
-    <t>Recherche de post qui aurait la même erreur. Rien de probant trouver.</t>
   </si>
   <si>
     <t>Poursuite du rapport de conception et modification de la schématisation réseau. Recheches sur plusieurs protocoles.</t>
@@ -475,9 +380,6 @@
     </r>
   </si>
   <si>
-    <t>Révision du câblage. UID récupérer. Le problème venait du cable qui était relier au port "IRQ".</t>
-  </si>
-  <si>
     <t>Recherches sur la récupération de données SQL dans une listbox et mise en place avec la fenêtre d'envoi d'indice à l'afficheur. Il est désormais possible de selectionner un indice prédéfini (actualisation systématique) et d'en créer un nouveau (enregistrer après envoi).</t>
   </si>
   <si>
@@ -529,9 +431,6 @@
     <t>Rédaction du rapport de conception.</t>
   </si>
   <si>
-    <t>Reception des jumpers manquant pour faire correctement les tests. Test du programme pour le module relais (programme tourne correctement mais aucun son de déclanchement entendu). Branchement de deux lecteur RFID et test des deux lecteurs, seul le premier branché fonctionne. Recherche sur les thread en python asynchrone qui permettrait de n'avoir aucune boucle "d'écoute" bloquante.</t>
-  </si>
-  <si>
     <t>Développement de l'esthétisme et de quelques améliorations de la page web et rédaction du rapport</t>
   </si>
   <si>
@@ -580,12 +479,6 @@
     <t>Apport de modifications sur le tableau de classement des équipes en fin de partie. Création d'une nouvelle fenêtre de type "A propos". Création d'un choix de nombre de joueurs sur la fenêtre de lancement et liaison avec la base de données.</t>
   </si>
   <si>
-    <t>Finalisations des premières version des rapport + recherche sur la différentiation des lecteurs RFID</t>
-  </si>
-  <si>
-    <t>Recherche sur la différentiation des lecteurs RFID</t>
-  </si>
-  <si>
     <t>Récupération de l'id du superviseur qui modifie un créneau (toujour en cours)</t>
   </si>
   <si>
@@ -622,12 +515,6 @@
     <t>Rédaction rapport</t>
   </si>
   <si>
-    <t>Recherche sur le changement du pin de contrôle du lecteur RFID</t>
-  </si>
-  <si>
-    <t>Recherche sur le changement du pin de contrôle du lecteur RFID + recherche sur comment controler les deux lecteurs en même temps</t>
-  </si>
-  <si>
     <t>Poursuite du rapport de conception (principalement sur la partie application). Etude de potentielles fiches recettes en fonction du diagramme de cas d'utilisation. Création et validation d'un test unitaire.</t>
   </si>
   <si>
@@ -652,9 +539,6 @@
     <t>Allumage des LEDs en simultané fonctionnel sans clignotement + réduction du code avec une fonction</t>
   </si>
   <si>
-    <t xml:space="preserve">La fonction ne fonctionne que pour la première qui est appelé + Test d'appelé les fonction en thread, aucun changement du comportement initiale + déclenchement du module relais si les deux UID sont valide + Confirmation de la nécéssite d'utilisé un deuxième bus spi  </t>
-  </si>
-  <si>
     <t>Création du diaporama de revue finale. Mise en place et préparation de la revue.</t>
   </si>
   <si>
@@ -664,10 +548,134 @@
     <t>Reflexions de calcul du pourcentage de reussite avec MySQL.</t>
   </si>
   <si>
-    <t>Activation du SPI1 + rajout du lecteur 3 +  déclenchement du module relais et du client socket (mit en commentraire car bloquant si le serveur socket n'est pas actif) si les trois UID sont valide + Lancement du programme au boot de la raspberry</t>
-  </si>
-  <si>
-    <t>PASSAGE REVUE FINAL</t>
+    <t>Poursuite du diaporama de revue finale et entrainement de passage à l'oral. Adaptation de la partie physique appliquée pour l'oral.</t>
+  </si>
+  <si>
+    <t>PASSAGE REVUE FINALE</t>
+  </si>
+  <si>
+    <t>Création du word pour la revue de projet n°1 et début de sa rédaction (perte du travail, mauvaise utilisation du Git) ; Choix d'un IDE, choix de Pycharm.</t>
+  </si>
+  <si>
+    <t>Création d'un journal d'activités commun ; Rédaction du word revue de projet n°1 ; Rédaction du Gantt commun</t>
+  </si>
+  <si>
+    <t>Rédaction des définitions de l'étudiant 1</t>
+  </si>
+  <si>
+    <t>Création du diaporama pour la revue de projet 1 + Rédaction des définitions de l'étudiant 1</t>
+  </si>
+  <si>
+    <t>Recherches bus SPI</t>
+  </si>
+  <si>
+    <t>Création d'un "Fritzing" (modèle de cablage) sur une platine d'essai + apport Gantt</t>
+  </si>
+  <si>
+    <t>Diagramme de séquence + recherches pour client/server socket</t>
+  </si>
+  <si>
+    <t>Travail sur l'ébauche de l'application.</t>
+  </si>
+  <si>
+    <t>Recherches pour client/server socket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalisation du diagramme de séquence pour le serveur socket asynchrone + préparation du diapo pour la revue 2 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Passage à la revue 2</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Poursuite du diaporama de revue. Poursuite et reinterprétation des analyses UML. Début de l'installation de DEBIAN (erreur carte SD à formatée en ligne de commandes) -&gt; Debian non installé.</t>
+    </r>
+  </si>
+  <si>
+    <t>Installation de raspbian + activation de du bus spi, port GPIO + installation de l'IDE phychram(problème d'installation, non finalisée)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résolution de l'erreur d'installation (installation pycharm complete) + installation de jdk </t>
+  </si>
+  <si>
+    <t>Tentative de récupération de l'uid (bug clavier, rend la navigation difficile) + Installation d'Anydesk pour une prise en main facilisée</t>
+  </si>
+  <si>
+    <t>Tentative de récupération de l'uid (difficulté de récupération des fonctions de la librairie)</t>
+  </si>
+  <si>
+    <t>Résolution de problème lié à la librairie et de son emplacement pour que le programme puisse y avoir accès.</t>
+  </si>
+  <si>
+    <t>Programme ne se lance pas avec le message d'erreur suivant "python: can't open file 'RecupUID.py': [Errno 2] No such file or directory".</t>
+  </si>
+  <si>
+    <t>Programme ne se lance pas avec même message d'erreur suivant "python: can't open file 'RecupUID.py': [Errno 2] No such file or directory".</t>
+  </si>
+  <si>
+    <t>Identification du problème des librairies avec la fonction "wait_for_tag" qui pose problème.</t>
+  </si>
+  <si>
+    <t>Recherches dans les différents chemins de fichier pour trouver l'origine du problème lié à l'erreur.</t>
+  </si>
+  <si>
+    <t>Recherches de posts qui auraient la même erreur. Rien de probant trouver.</t>
+  </si>
+  <si>
+    <t>Révision du câblage. UID récupéré. Le problème venait du cable qui était relié au port "IRQ".</t>
+  </si>
+  <si>
+    <t>Reception des jumpers manquant pour faire correctement les tests. Test du programme pour le module relais (programme tourne correctement mais aucun son de déclanchement entendu). Branchement de deux lecteurs RFID et test des deux lecteurs, seul le premier branché fonctionne. Recherche sur les thread en python asynchrone qui permettrait de n'avoir aucune boucle "d'écoute" bloquante.</t>
+  </si>
+  <si>
+    <t>Finalisations des premières versions des rapport + recherches sur la différentiation des lecteurs RFID</t>
+  </si>
+  <si>
+    <t>Recherches sur la différentiation des lecteurs RFID</t>
+  </si>
+  <si>
+    <t>Recherches sur le changement du pin de contrôle du lecteur RFID</t>
+  </si>
+  <si>
+    <t>Recherches sur le changement du pin de contrôle du lecteur RFID + recherche sur comment controler les deux lecteurs en même temps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La fonction ne fonctionne que pour la première qui est appelé + Test d'appel des fonctions en thread, aucun changement du comportement initial + déclenchement du module relais si les deux UID sont valide + Confirmation de la nécéssite d'utiliser un deuxième bus spi  </t>
+  </si>
+  <si>
+    <t>Activation du SPI1 + rajout du lecteur 3 +  déclenchement du module relais et du client socket (mis en commentraire car bloquant si le serveur socket n'est pas actif) si les trois UID sont valide + Lancement du programme au boot de la raspberry</t>
+  </si>
+  <si>
+    <t>Recherches et aide pour la récupération de l'image provenant de la caméra IP pour le code en C#. Poursuite de la configuration de la caméra IP et création d'un compte MyDlink</t>
+  </si>
+  <si>
+    <t>Poursuite des diagrammes de séquence. Création d'un modèle relationnel pour la base de données. Création d'un diagramme de classes pour l'application de supervision. Renseignement sur fonction "singleton" en C#. Re-définition des besoins en matière de base de données.</t>
+  </si>
+  <si>
+    <t>Application de supervision : Etude de la connexion avec la base de données (tutoriel) et début de mise en œuvre pour la fenêtre d'envoi d'indice. Résolution d'un problème avec une surcharge de Teams rendant impossible l'utilisation de Visual Studio (30 min).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poursuite des tests et approfondissement de la communication entre la base de données et l'application. Extraction du script de la BDD. Recherches et tests (implémentation) de code pour l'affichage du chronometre dans la fenêtre principale. </t>
+  </si>
+  <si>
+    <t>Recherches et création d'une requête SQL permettant d'insérer l'heure de fin de partie dans le dernier enregistrement (correspondant à l'équipe en cours). Mise en place dans l'application et tests validés. Création d'une méthode de mise à jour du score en fin de partie, non terminée.</t>
   </si>
 </sst>
 </file>
@@ -677,7 +685,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -748,14 +756,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -772,8 +772,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -799,7 +814,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -887,7 +908,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -913,12 +934,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -931,19 +946,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -955,10 +967,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1282,45 +1309,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B148" sqref="B148"/>
+    <sheetView tabSelected="1" topLeftCell="B142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="14"/>
+    <col min="1" max="1" width="11.42578125" style="12"/>
     <col min="2" max="2" width="49.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="16"/>
+    <col min="4" max="4" width="11.42578125" style="13"/>
     <col min="5" max="5" width="44.85546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="16"/>
-    <col min="8" max="8" width="42.5703125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="13"/>
+    <col min="8" max="8" width="42.5703125" style="17" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="17"/>
+    <col min="10" max="10" width="11.42578125" style="14"/>
     <col min="11" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1329,19 +1356,19 @@
         <v>43844</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>0.125</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="6">
         <v>0.125</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I2" s="1">
         <v>0.125</v>
@@ -1352,19 +1379,19 @@
         <v>43845</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>6</v>
+        <v>148</v>
       </c>
       <c r="C3" s="1">
         <v>0.13541666666666666</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="6">
         <v>0.125</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I3" s="1">
         <v>0.125</v>
@@ -1381,19 +1408,19 @@
         <v>43847</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>149</v>
       </c>
       <c r="C5" s="1">
         <v>0.20833333333333334</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5" s="6">
         <v>0.20833333333333334</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1">
         <v>0.20833333333333334</v>
@@ -1425,19 +1452,19 @@
         <v>43851</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F9" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="I9" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1448,19 +1475,19 @@
         <v>43852</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>17</v>
+        <v>150</v>
       </c>
       <c r="C10" s="1">
         <v>0.125</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F10" s="6">
         <v>0.125</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="I10" s="1">
         <v>0.125</v>
@@ -1501,19 +1528,19 @@
         <v>43858</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>151</v>
       </c>
       <c r="C16" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F16" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="I16" s="1">
         <v>0.16666666666666666</v>
@@ -1524,19 +1551,19 @@
         <v>43859</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F17" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="I17" s="1">
         <v>4.1666666666666664E-2</v>
@@ -1553,13 +1580,13 @@
         <v>43861</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1">
         <v>0.125</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F19" s="6">
         <v>0.125</v>
@@ -1591,19 +1618,19 @@
         <v>43865</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F23" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="I23" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1614,19 +1641,19 @@
         <v>43866</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>27</v>
+        <v>152</v>
       </c>
       <c r="C24" s="1">
         <v>0.125</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F24" s="6">
         <v>0.125</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I24" s="1">
         <v>0.125</v>
@@ -1643,19 +1670,19 @@
         <v>43868</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>153</v>
       </c>
       <c r="C26" s="1">
         <v>0.2638888888888889</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F26" s="6">
-        <v>0.25</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I26" s="1">
         <v>0.25</v>
@@ -1684,19 +1711,19 @@
         <v>43872</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C30" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>31</v>
+        <v>177</v>
       </c>
       <c r="F30" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="I30" s="1">
         <v>0.16666666666666666</v>
@@ -1707,19 +1734,19 @@
         <v>43873</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C31" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F31" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="I31" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1736,19 +1763,19 @@
         <v>43875</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>34</v>
+        <v>154</v>
       </c>
       <c r="C33" s="1">
         <v>0.25</v>
       </c>
       <c r="E33" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H33" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="F33" s="6">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="I33" s="1">
         <v>0.25</v>
@@ -1783,6 +1810,12 @@
         <v>43880</v>
       </c>
       <c r="B38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F38" s="6">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
@@ -1827,7 +1860,7 @@
       <c r="B45" s="5"/>
       <c r="C45" s="1"/>
       <c r="E45" s="5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F45" s="6">
         <v>8.3333333333333329E-2</v>
@@ -1839,7 +1872,7 @@
         <v>43888</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C46" s="1">
         <v>6.25E-2</v>
@@ -1874,19 +1907,19 @@
         <v>43893</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>52</v>
+        <v>156</v>
       </c>
       <c r="C51" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F51" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="I51" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1897,19 +1930,19 @@
         <v>43894</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>52</v>
+        <v>156</v>
       </c>
       <c r="C52" s="1">
         <v>0.125</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F52" s="6">
         <v>0.125</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="I52" s="1">
         <v>0.125</v>
@@ -1925,20 +1958,20 @@
       <c r="A54" s="3">
         <v>43896</v>
       </c>
-      <c r="B54" s="15" t="s">
-        <v>51</v>
+      <c r="B54" s="5" t="s">
+        <v>157</v>
       </c>
       <c r="C54" s="1">
         <v>0.25</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F54" s="6">
         <v>0.25</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I54" s="1">
         <v>0.25</v>
@@ -1967,19 +2000,19 @@
         <v>43900</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C58" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E58" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F58" s="6">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H58" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="F58" s="6">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="I58" s="1">
         <v>0.16666666666666666</v>
@@ -1990,19 +2023,19 @@
         <v>43901</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C59" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F59" s="6">
         <v>0.125</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="I59" s="1">
         <v>8.3333333333333329E-2</v>
@@ -2018,20 +2051,20 @@
       <c r="A61" s="3">
         <v>43903</v>
       </c>
-      <c r="B61" s="7" t="s">
-        <v>57</v>
+      <c r="B61" s="5" t="s">
+        <v>158</v>
       </c>
       <c r="C61" s="1">
         <v>0.25</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="F61" s="6">
         <v>0.25</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I61" s="1">
         <v>0.25</v>
@@ -2055,13 +2088,13 @@
       </c>
       <c r="B64" s="5"/>
       <c r="E64" s="5" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F64" s="6">
         <v>0.14583333333333334</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="I64" s="1">
         <v>0.16666666666666666</v>
@@ -2072,19 +2105,19 @@
         <v>43907</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="C65" s="1">
         <v>0.125</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F65" s="6">
         <v>0.1875</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="I65" s="1">
         <v>0.20833333333333334</v>
@@ -2095,19 +2128,19 @@
         <v>43908</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C66" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="F66" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="I66" s="1">
         <v>8.3333333333333329E-2</v>
@@ -2119,13 +2152,13 @@
       </c>
       <c r="B67" s="5"/>
       <c r="E67" s="5" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F67" s="6">
         <v>0.125</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="I67" s="1">
         <v>0.16666666666666666</v>
@@ -2136,13 +2169,13 @@
         <v>43910</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="C68" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="F68" s="6">
         <v>0.16666666666666666</v>
@@ -2165,19 +2198,19 @@
         <v>43913</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C71" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="F71" s="6">
         <v>0.125</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="I71" s="1">
         <v>6.25E-2</v>
@@ -2188,19 +2221,19 @@
         <v>43914</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="C72" s="1">
         <v>0.125</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>78</v>
+        <v>179</v>
       </c>
       <c r="F72" s="6">
         <v>0.125</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="I72" s="1">
         <v>0.20833333333333334</v>
@@ -2212,13 +2245,13 @@
       </c>
       <c r="B73" s="5"/>
       <c r="E73" s="5" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F73" s="6">
-        <v>0.16666666666666666</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="I73" s="1">
         <v>8.3333333333333329E-2</v>
@@ -2229,19 +2262,19 @@
         <v>43916</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="C74" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="F74" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="I74" s="1">
         <v>0.20833333333333334</v>
@@ -2252,19 +2285,19 @@
         <v>43917</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>97</v>
+        <v>163</v>
       </c>
       <c r="C75" s="1">
         <v>0.125</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="F75" s="6">
         <v>0.1875</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="I75" s="1">
         <v>0.125</v>
@@ -2287,19 +2320,19 @@
         <v>43920</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>99</v>
+        <v>164</v>
       </c>
       <c r="C78" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="F78" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="I78" s="1">
         <v>8.3333333333333329E-2</v>
@@ -2310,19 +2343,19 @@
         <v>43921</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>100</v>
+        <v>165</v>
       </c>
       <c r="C79" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>89</v>
+        <v>181</v>
       </c>
       <c r="F79" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2331,13 +2364,13 @@
       </c>
       <c r="B80" s="5"/>
       <c r="E80" s="5" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="F80" s="6">
         <v>0.10416666666666667</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="I80" s="1">
         <v>0.125</v>
@@ -2355,19 +2388,19 @@
         <v>43924</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>98</v>
+        <v>166</v>
       </c>
       <c r="C82" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F82" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="I82" s="1">
         <v>0.125</v>
@@ -2391,19 +2424,19 @@
         <v>43927</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>101</v>
+        <v>167</v>
       </c>
       <c r="C85" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="F85" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="I85" s="1">
         <v>0.16666666666666666</v>
@@ -2414,19 +2447,19 @@
         <v>43928</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="C86" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="F86" s="6">
-        <v>0.10416666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="I86" s="1">
         <v>0.16666666666666666</v>
@@ -2437,19 +2470,19 @@
         <v>43929</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="C87" s="1">
         <v>0.125</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="F87" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="I87" s="1">
         <v>0.125</v>
@@ -2460,19 +2493,19 @@
         <v>43930</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="C88" s="1">
         <v>0.125</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="F88" s="6">
         <v>0.10416666666666667</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="I88" s="1">
         <v>0.20833333333333334</v>
@@ -2483,19 +2516,19 @@
         <v>43931</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="C89" s="1">
-        <v>0.14583333333333334</v>
+        <v>0.125</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="F89" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="H89" s="20" t="s">
-        <v>140</v>
+      <c r="H89" s="17" t="s">
+        <v>113</v>
       </c>
       <c r="I89" s="1">
         <v>0.125</v>
@@ -2518,15 +2551,15 @@
         <v>43934</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>115</v>
+        <v>169</v>
       </c>
       <c r="C92" s="1">
         <v>0.20833333333333334</v>
       </c>
-      <c r="E92" s="21"/>
-      <c r="F92" s="22"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="19"/>
       <c r="H92" s="5" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="I92" s="1">
         <v>0.20833333333333334</v>
@@ -2537,13 +2570,13 @@
         <v>43935</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="C93" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="F93" s="6">
         <v>0.16666666666666666</v>
@@ -2554,13 +2587,13 @@
         <v>43936</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="C94" s="1">
         <v>0.20833333333333334</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="F94" s="6">
         <v>0.16666666666666666</v>
@@ -2572,13 +2605,13 @@
       </c>
       <c r="B95" s="5"/>
       <c r="E95" s="5" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="F95" s="6">
         <v>0.1875</v>
       </c>
-      <c r="H95" s="20" t="s">
-        <v>142</v>
+      <c r="H95" s="17" t="s">
+        <v>115</v>
       </c>
       <c r="I95" s="1">
         <v>0.125</v>
@@ -2590,13 +2623,13 @@
       </c>
       <c r="B96" s="5"/>
       <c r="E96" s="5" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="F96" s="6">
         <v>0.1875</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="I96" s="1">
         <v>0.20833333333333334</v>
@@ -2619,19 +2652,19 @@
         <v>43941</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="C99" s="1">
         <v>0.125</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="F99" s="6">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H99" s="20" t="s">
-        <v>138</v>
+      <c r="H99" s="17" t="s">
+        <v>111</v>
       </c>
       <c r="I99" s="1">
         <v>0.125</v>
@@ -2642,19 +2675,19 @@
         <v>43942</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="C100" s="1">
         <v>0.125</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="F100" s="6">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H100" s="20" t="s">
-        <v>137</v>
+      <c r="H100" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="I100" s="1">
         <v>0.125</v>
@@ -2665,19 +2698,19 @@
         <v>43943</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="C101" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="F101" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="I101" s="1">
         <v>0.125</v>
@@ -2688,19 +2721,19 @@
         <v>43944</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="C102" s="1">
         <v>0.14583333333333334</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="F102" s="6">
         <v>0.10416666666666667</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="I102" s="1">
         <v>0.20833333333333334</v>
@@ -2711,19 +2744,19 @@
         <v>43945</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="C103" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="F103" s="6">
         <v>0.10416666666666667</v>
       </c>
       <c r="H103" s="5" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="I103" s="1">
         <v>0.20833333333333334</v>
@@ -2746,19 +2779,19 @@
         <v>43948</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="C106" s="1">
         <v>0.20833333333333334</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="F106" s="6">
         <v>0.1875</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="I106" s="1">
         <v>0.20833333333333334</v>
@@ -2769,19 +2802,19 @@
         <v>43949</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="C107" s="1">
         <v>0.25</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="F107" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="I107" s="1">
         <v>0.20833333333333334</v>
@@ -2792,19 +2825,19 @@
         <v>43950</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="C108" s="1">
         <v>0.39583333333333331</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="F108" s="6">
         <v>0.1875</v>
       </c>
       <c r="H108" s="5" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="I108" s="1">
         <v>0.125</v>
@@ -2815,19 +2848,19 @@
         <v>43951</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="C109" s="1">
         <v>0.125</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="F109" s="6">
         <v>0.25</v>
       </c>
-      <c r="H109" s="20" t="s">
-        <v>145</v>
+      <c r="H109" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="I109" s="1">
         <v>0.20833333333333334</v>
@@ -2838,19 +2871,19 @@
         <v>43952</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="C110" s="1">
         <v>0.20833333333333334</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="F110" s="6">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H110" s="20" t="s">
-        <v>145</v>
+      <c r="H110" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="I110" s="1">
         <v>0.20833333333333334</v>
@@ -2861,19 +2894,19 @@
         <v>43953</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="C111" s="1">
         <v>0.25</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="F111" s="6">
         <v>0.10416666666666667</v>
       </c>
-      <c r="H111" s="20" t="s">
-        <v>145</v>
+      <c r="H111" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="I111" s="1">
         <v>0.125</v>
@@ -2884,13 +2917,13 @@
         <v>43954</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="C112" s="1">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H112" s="20" t="s">
-        <v>145</v>
+      <c r="H112" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="I112" s="1">
         <v>8.3333333333333329E-2</v>
@@ -2901,19 +2934,19 @@
         <v>43955</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="C113" s="1">
         <v>0.1875</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="F113" s="6">
         <v>0.1875</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="I113" s="1">
         <v>0.20833333333333334</v>
@@ -2924,19 +2957,19 @@
         <v>43956</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="C114" s="1">
         <v>0.15277777777777776</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="F114" s="6">
         <v>0.10416666666666667</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="I114" s="1">
         <v>0.16666666666666666</v>
@@ -2948,13 +2981,13 @@
       </c>
       <c r="B115" s="5"/>
       <c r="E115" s="5" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="F115" s="6">
         <v>0.125</v>
       </c>
       <c r="H115" s="5" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="I115" s="1">
         <v>0.16666666666666666</v>
@@ -2965,19 +2998,19 @@
         <v>43958</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C116" s="1">
         <v>0.125</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="F116" s="6">
         <v>0.14583333333333334</v>
       </c>
       <c r="H116" s="5" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="I116" s="1">
         <v>0.20833333333333334</v>
@@ -2988,7 +3021,7 @@
         <v>43959</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C117" s="1">
         <v>0.20833333333333334</v>
@@ -3011,19 +3044,19 @@
         <v>43962</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C120" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="F120" s="6">
         <v>0.125</v>
       </c>
-      <c r="H120" s="20" t="s">
-        <v>160</v>
+      <c r="H120" s="17" t="s">
+        <v>131</v>
       </c>
       <c r="I120" s="1">
         <v>0.125</v>
@@ -3034,19 +3067,19 @@
         <v>43963</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C121" s="1">
         <v>0.20833333333333334</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="F121" s="6">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H121" s="20" t="s">
-        <v>162</v>
+      <c r="H121" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="I121" s="1">
         <v>0.125</v>
@@ -3057,19 +3090,19 @@
         <v>43964</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C122" s="1">
         <v>0.20833333333333334</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="F122" s="6">
         <v>0.22916666666666666</v>
       </c>
-      <c r="H122" s="20" t="s">
-        <v>159</v>
+      <c r="H122" s="17" t="s">
+        <v>130</v>
       </c>
       <c r="I122" s="1">
         <v>0.20833333333333334</v>
@@ -3080,13 +3113,13 @@
         <v>43965</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C123" s="1">
         <v>0.1875</v>
       </c>
-      <c r="H123" s="20" t="s">
-        <v>172</v>
+      <c r="H123" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="I123" s="1">
         <v>0.1875</v>
@@ -3097,19 +3130,19 @@
         <v>43966</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C124" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="F124" s="6">
         <v>0.27083333333333331</v>
       </c>
-      <c r="H124" s="20" t="s">
-        <v>172</v>
+      <c r="H124" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="I124" s="1">
         <v>0.16666666666666666</v>
@@ -3120,7 +3153,7 @@
         <v>43967</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C125" s="1">
         <v>0.20833333333333334</v>
@@ -3131,7 +3164,7 @@
         <v>43968</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C126" s="1">
         <v>0.25</v>
@@ -3142,19 +3175,19 @@
         <v>43969</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C127" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="F127" s="6">
         <v>0.14583333333333334</v>
       </c>
-      <c r="H127" s="20" t="s">
-        <v>172</v>
+      <c r="H127" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="I127" s="1">
         <v>0.125</v>
@@ -3165,13 +3198,13 @@
         <v>43970</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C128" s="1">
         <v>0.125</v>
       </c>
-      <c r="H128" s="20" t="s">
-        <v>172</v>
+      <c r="H128" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="I128" s="1">
         <v>8.3333333333333329E-2</v>
@@ -3212,7 +3245,7 @@
         <v>43976</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="C134" s="1">
         <v>0.16666666666666666</v>
@@ -3223,7 +3256,7 @@
         <v>43977</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="C135" s="1">
         <v>0.16666666666666666</v>
@@ -3234,7 +3267,7 @@
         <v>43978</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="C136" s="1">
         <v>0.20833333333333334</v>
@@ -3245,13 +3278,13 @@
         <v>43979</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="C137" s="1">
         <v>0.125</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="F137" s="6">
         <v>8.3333333333333329E-2</v>
@@ -3262,13 +3295,13 @@
         <v>43980</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="C138" s="1">
         <v>0.29166666666666669</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="F138" s="6">
         <v>0.125</v>
@@ -3291,7 +3324,7 @@
         <v>43983</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C141" s="1">
         <v>0.33333333333333331</v>
@@ -3302,23 +3335,29 @@
         <v>43984</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C142" s="1">
         <v>0.29166666666666669</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="F142" s="6">
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>43985</v>
       </c>
       <c r="B143" s="5"/>
+      <c r="E143" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F143" s="6">
+        <v>0.16666666666666666</v>
+      </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
@@ -3350,18 +3389,28 @@
       </c>
       <c r="B148" s="5"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>43991</v>
       </c>
       <c r="B149" s="23" t="s">
-        <v>179</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="C149" s="20">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D149" s="22"/>
       <c r="E149" s="23" t="s">
-        <v>179</v>
+        <v>147</v>
+      </c>
+      <c r="F149" s="21">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="H149" s="24" t="s">
-        <v>179</v>
+        <v>147</v>
+      </c>
+      <c r="I149" s="20">
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -3402,19 +3451,19 @@
     </row>
     <row r="159" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C159" s="9">
+        <v>6</v>
+      </c>
+      <c r="C159" s="25">
         <f>SUM(C2:C155)</f>
-        <v>11.23958333333333</v>
-      </c>
-      <c r="F159" s="9">
+        <v>11.260416666666664</v>
+      </c>
+      <c r="F159" s="25">
         <f>SUM(F2:F155)</f>
-        <v>9.9583333333333375</v>
-      </c>
-      <c r="I159" s="10">
+        <v>10.375000000000002</v>
+      </c>
+      <c r="I159" s="26">
         <f>SUM(I2:I155)</f>
-        <v>9.6249999999999982</v>
+        <v>9.6666666666666643</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finalisation de la correction de l'orthographe du journal d'activités.
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A6933A-FBB2-4181-ADF9-68DCA742D13B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A8E973-8031-4AF5-A0D8-899DB9A87E50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="183">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -74,18 +74,9 @@
     <t>Poursuite du diagramme de séquence propre à l'application de supervision souhaitée.</t>
   </si>
   <si>
-    <t>Lancement du projet : Annalyse du dossier, création du GitHub (GitKraken),  recherche d'information sur Boostrap et Apache. Debut de rédaction de mon document Word de documentation</t>
-  </si>
-  <si>
-    <t>Recherche d'information sur le developpement sur Arduino et sur le materiel (buzzer, écran LCD). Poursuite de la rédaction de mon fichier word.</t>
-  </si>
-  <si>
     <t>Création du diaporama support pour la revue 1. Pousuite du diagramme de séquences. Poursuite du dossier étudiant.</t>
   </si>
   <si>
-    <t>Rédaction d'un Gantt commun. Rédaction de mon diaporama pour la revu de projet n°1. Poursuite de la rédaction de mon fichier word.</t>
-  </si>
-  <si>
     <t>Poursuite du diaporama support pour la revue 1. Analyse sous forme de diagramme de séquence.</t>
   </si>
   <si>
@@ -110,23 +101,6 @@
     <t xml:space="preserve">Finalisation du câble sur Fritzing + adaptation du câble pour les LEDs + revue du diagrame de séquence </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Finalisation du diagramme de Gantt, ainsi que de la revue. 1 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Passage à la revue 1</t>
-    </r>
-  </si>
-  <si>
     <t>Diagramme de séquence</t>
   </si>
   <si>
@@ -142,12 +116,6 @@
     <t>Création du chemin de fer et mise à jour du diaporama.</t>
   </si>
   <si>
-    <t>Puirsuite des recherches, de la rédaction du diaporama et de la rédaction de la documentation.</t>
-  </si>
-  <si>
-    <t>Mise a jour de mon diaporama, poursuite des recherches.</t>
-  </si>
-  <si>
     <t>Mise à jour du Gantt et création du diagramme de séquence pour l'application arduino.</t>
   </si>
   <si>
@@ -161,9 +129,6 @@
   </si>
   <si>
     <t>Recherche d'éléments pour naviguer facilement pour la page web et recherche cablage pour l'application arduino</t>
-  </si>
-  <si>
-    <t>Réflexion général sur mes deux parties</t>
   </si>
   <si>
     <t>Mise à jour du diagramme de Gantt. Poursuite du diaporama de revue 2. Mise à jour des diagrammes de séquence et mise en commun de certaines parties avec Guillaume.</t>
@@ -224,18 +189,9 @@
     <t xml:space="preserve">Finalisation de la configuration de Visual Studio. Poursuite de l'application de supervision. Etude approfondie de l'adaptateur RS232 - Wi-Fi (en parallèle avec un travail en ESLA sur ce même adaptateur). </t>
   </si>
   <si>
-    <t>Correction des diagrammes de sèquences et de classes, poursuite des modification du diaporama pour la revue 2.</t>
-  </si>
-  <si>
     <t>Programmation du Menu du site web et amorce de la page de connexion.</t>
   </si>
   <si>
-    <t>Amorce du ablage de l'arduino avec ces differents composants et amorce de la programmation sur l'arduino.</t>
-  </si>
-  <si>
-    <t>Poursuite des modifications du diaporama, finalisation des diragrammes, ajout des documentation sur le gantt.</t>
-  </si>
-  <si>
     <t>Maquette du Cablage de l'ensemble de l'application arduino</t>
   </si>
   <si>
@@ -248,12 +204,6 @@
     <t>Poursuite de l'application de supervision. Travail et étude sur la trame et la méthode pour l'envoyée à l'afficheur.</t>
   </si>
   <si>
-    <t>Programmation de la page de connexion. Recherche comment avoir deux mots de passe differents pour deux pages differentes</t>
-  </si>
-  <si>
-    <t>Programmation de la page d'administrateur, recherche comment supprimer, ajouter, modifier la bdd depuis la page web</t>
-  </si>
-  <si>
     <t>Tentative de résolution de l'erreur</t>
   </si>
   <si>
@@ -308,12 +258,6 @@
     <t>Création des bases pour les rapports d'analyse et de conception communs. Recherches et tests de plusieurs méthodes avec DATASET pour classer les résultats d'une requête SQL dans un tableau de la fenêtre. Recherches non abouties.</t>
   </si>
   <si>
-    <t>mise à jour bdd, programmation sur l'application Arduino</t>
-  </si>
-  <si>
-    <t>Programmation Lien entre ajout de créneaux et calendrier</t>
-  </si>
-  <si>
     <t>Poursuite des recherches pour la récupération de la requête SQL dans un tableau C#. Non aboutissement de celles-ci.</t>
   </si>
   <si>
@@ -324,15 +268,6 @@
   </si>
   <si>
     <t>Poursuite du rapport de conception et modification de la schématisation réseau. Recheches sur plusieurs protocoles.</t>
-  </si>
-  <si>
-    <t>Programmation d'un événement cliquable et d'une page de résérvation de créneaux avec les informations du créneau cliqué</t>
-  </si>
-  <si>
-    <t>Programmation Arduino, connexion de tous les composants + programme permettant d'activer buzzer et afficheur lcd  quand le bon code est rentré</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Programmation site web en général, nettyage, esthétique </t>
   </si>
   <si>
     <t>Poursuite des recherches et nouveaux tests pour la récupération des résultats de la requête SQL dans un tableau.</t>
@@ -363,26 +298,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Mise au point de l'oral. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Passage de la revue 1</t>
-    </r>
-  </si>
-  <si>
-    <t>Recherches sur la récupération de données SQL dans une listbox et mise en place avec la fenêtre d'envoi d'indice à l'afficheur. Il est désormais possible de selectionner un indice prédéfini (actualisation systématique) et d'en créer un nouveau (enregistrer après envoi).</t>
-  </si>
-  <si>
     <t>Création d'un programme pour l'allumage de la led si l'uid est valide. UID est bien prit en compte mais la LED ne s'allume pas. Mettre plusieurs lecteurs RFID impossible car il y un manque de cables.</t>
   </si>
   <si>
@@ -416,9 +331,6 @@
     <t>Création de deux textblock permettant de récupérer le dernier indice envoyé à la base de données ainsi que l'équipe en cours. Affichage de ces deux données sur la fenêtre principale. Tentative de configuration de l'adaptateur et demande d'aide mais sans succès.</t>
   </si>
   <si>
-    <t>Modifications des interfaces graphiques de l'application et poursuite de la récupération du nom de l'équipe et du dernier indice envoyé. Réalisation de tests de l'ensemble des fonctions.</t>
-  </si>
-  <si>
     <t>Poursuite du rapport de conception et étude de certains élements pour présentation. Apport de quelques corrections sur l'application de supervision avec l'aide en Visio de Monsieur HOURDIN. Changement des paramètres de la fenêtre de confirmation de fin de partie et création d'une fonction "Terminer Partie()" auquel Guillaume pourra déposer la partie Socket Client-Serveur.</t>
   </si>
   <si>
@@ -434,33 +346,15 @@
     <t>Développement de l'esthétisme et de quelques améliorations de la page web et rédaction du rapport</t>
   </si>
   <si>
-    <t>Développement des exigences du système, essaie de récuperer l'id du superviseur qui modifie, supprime ou ajoute un créneau</t>
-  </si>
-  <si>
-    <t>Poursuite du développement des exigences du système et de la rédaction du rapport</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nettoyage de NetBeans </t>
   </si>
   <si>
     <t>Rédaction du rapport</t>
   </si>
   <si>
-    <t>Poursuite de la rédaction du rapport et programmation de la musique au claire de la lune du buzzer</t>
-  </si>
-  <si>
-    <t>Développement web, gestions créneaux</t>
-  </si>
-  <si>
-    <t>Développement  de la gestions utilisateur (admin et superviseur), rediréction en fonction du mot de passe</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rédaction du rapport </t>
   </si>
   <si>
-    <t>Résolution de quelques erreurs de programmation dans l'application de supervision. Poursuite du rapport de conception. Création de la structure complète du rapport d'analyse et de spécifications et intégration du diagramme de classe, des diagrmmes de séquences, présentation du projet dans celui-ci.</t>
-  </si>
-  <si>
     <t>Poursuite du rapport d'analyse et de spécification.</t>
   </si>
   <si>
@@ -479,16 +373,7 @@
     <t>Apport de modifications sur le tableau de classement des équipes en fin de partie. Création d'une nouvelle fenêtre de type "A propos". Création d'un choix de nombre de joueurs sur la fenêtre de lancement et liaison avec la base de données.</t>
   </si>
   <si>
-    <t>Récupération de l'id du superviseur qui modifie un créneau (toujour en cours)</t>
-  </si>
-  <si>
-    <t>Affichage d'une alert avec le numéro de téléphone quand le superviseur supprime un créneau réservé</t>
-  </si>
-  <si>
     <t>Faire en sorte de ne pas pouvoir inserer un creneaux déjà existant et qu'il y ai un minimum de 30 min entre les créneaux (toujours en cours)</t>
-  </si>
-  <si>
-    <t>Ecriture de commentaires dans le code. Reprise de certains boutons et trie des données dans la base de données. Point de projet.</t>
   </si>
   <si>
     <t>Commentage de la partie code. Poursuite du rapport de conception avec l'étude du réseau Wi-Fi pour la partie physique appliquée.</t>
@@ -677,6 +562,124 @@
   <si>
     <t>Recherches et création d'une requête SQL permettant d'insérer l'heure de fin de partie dans le dernier enregistrement (correspondant à l'équipe en cours). Mise en place dans l'application et tests validés. Création d'une méthode de mise à jour du score en fin de partie, non terminée.</t>
   </si>
+  <si>
+    <t>Recherches sur la récupération de données SQL dans une listbox et mise en place avec la fenêtre d'envoi d'indice à l'afficheur. Il est désormais possible de selectionner un indice prédéfini (actualisation systématique) et d'en créer un nouveau (enregistrement après envoi).</t>
+  </si>
+  <si>
+    <t>Modification des interfaces graphiques de l'application et poursuite de la récupération du nom de l'équipe et du dernier indice envoyé. Réalisation de tests de l'ensemble des fonctions.</t>
+  </si>
+  <si>
+    <t>Résolution de quelques erreurs de programmation dans l'application de supervision. Poursuite du rapport de conception. Création de la structure complète du rapport d'analyse et de spécifications et intégration du diagramme de classe, des diagrammes de séquences, présentation du projet dans celui-ci.</t>
+  </si>
+  <si>
+    <t>Ecriture de commentaires dans le code. Reprise de certains boutons et tri des données dans la base de données. Point de projet.</t>
+  </si>
+  <si>
+    <t>Lancement du projet : Annalyse du dossier, création du GitHub (GitKraken),  recherches d'informations sur Boostrap et Apache. Debut de rédaction de mon document Word de documentation.</t>
+  </si>
+  <si>
+    <t>Recherches d'informations sur le developpement sur Arduino et sur le materiel (buzzer, écran LCD). Poursuite de la rédaction de mon fichier word.</t>
+  </si>
+  <si>
+    <t>Rédaction d'un Gantt commun. Rédaction de mon diaporama pour la revue de projet n°1. Poursuite de la rédaction de mon fichier word.</t>
+  </si>
+  <si>
+    <t>Mise à jour de mon diaporama, poursuite des recherches.</t>
+  </si>
+  <si>
+    <t>Poursuite des recherches, de la rédaction du diaporama et de la rédaction de la documentation.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mise au point de l'oral. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Passage de la revue 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Finalisation du diagramme de Gantt, ainsi que de la revue. 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Passage de la revue 1</t>
+    </r>
+  </si>
+  <si>
+    <t>Réflexions générales sur mes deux parties</t>
+  </si>
+  <si>
+    <t>Poursuite des modifications du diaporama, finalisation des diragrammes, ajout des documentations sur le gantt.</t>
+  </si>
+  <si>
+    <t>Correction des diagrammes de séquences et de classes, poursuite des modification du diaporama pour la revue 2.</t>
+  </si>
+  <si>
+    <t>Amorce du cablage de l'arduino avec ses differents composants et amorce de la programmation sur l'arduino.</t>
+  </si>
+  <si>
+    <t>Programmation de la page de connexion. Recherches sur comment avoir deux mots de passe differents pour deux pages differentes</t>
+  </si>
+  <si>
+    <t>Programmation de la page d'administrateur, recherches de comment supprimer, ajouter, modifier la bdd depuis la page web</t>
+  </si>
+  <si>
+    <t>Mise à jour bdd, programmation sur l'application Arduino</t>
+  </si>
+  <si>
+    <t>Programmation du lien entre l'ajout de créneaux et le calendrier</t>
+  </si>
+  <si>
+    <t>Programmation d'un événement cliquable et d'une page de résérvation de créneaux avec les informations du créneau cliqué.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmation site web en général, nettyage, graphisme. </t>
+  </si>
+  <si>
+    <t>Programmation Arduino, connexion de tous les composants + programme permettant d'activer buzzer et afficheur lcd  quand le bon code est saisi.</t>
+  </si>
+  <si>
+    <t>Développement web, gestions de créneaux</t>
+  </si>
+  <si>
+    <t>Développement de l'esthétisme et de quelques améliorations de la page web et rédaction du rapport.</t>
+  </si>
+  <si>
+    <t>Développement de la gestion utilisateur (admin et superviseur), redirection en fonction du mot de passe.</t>
+  </si>
+  <si>
+    <t>Développement des exigences du système, essai de récuperer l'id du superviseur qui modifie, supprime ou ajoute un créneau.</t>
+  </si>
+  <si>
+    <t>Poursuite du développement des exigences du système et de la rédaction du rapport.</t>
+  </si>
+  <si>
+    <t>Poursuite de la rédaction du rapport et programmation de la musique "au claire de la lune" du buzzer</t>
+  </si>
+  <si>
+    <t>Récupération de l'id du superviseur qui modifie un créneau (toujours en cours)</t>
+  </si>
+  <si>
+    <t>Affichage d'une alerte avec le numéro de téléphone quand le superviseur supprime un créneau réservé</t>
+  </si>
 </sst>
 </file>
 
@@ -685,7 +688,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,15 +767,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="8"/>
       <name val="Calibri"/>
@@ -788,7 +782,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -809,12 +803,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -908,7 +896,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -961,32 +949,35 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1309,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E152" sqref="E152"/>
+    <sheetView tabSelected="1" topLeftCell="B144" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E157" sqref="E157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1359,7 @@
         <v>0.125</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="I2" s="1">
         <v>0.125</v>
@@ -1379,7 +1370,7 @@
         <v>43845</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1">
         <v>0.13541666666666666</v>
@@ -1391,7 +1382,7 @@
         <v>0.125</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="I3" s="1">
         <v>0.125</v>
@@ -1408,7 +1399,7 @@
         <v>43847</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="C5" s="1">
         <v>0.20833333333333334</v>
@@ -1420,7 +1411,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>16</v>
+        <v>159</v>
       </c>
       <c r="I5" s="1">
         <v>0.20833333333333334</v>
@@ -1464,7 +1455,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I9" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1475,19 +1466,19 @@
         <v>43852</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="C10" s="1">
         <v>0.125</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F10" s="6">
         <v>0.125</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>32</v>
+        <v>160</v>
       </c>
       <c r="I10" s="1">
         <v>0.125</v>
@@ -1528,19 +1519,19 @@
         <v>43858</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="C16" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F16" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>31</v>
+        <v>161</v>
       </c>
       <c r="I16" s="1">
         <v>0.16666666666666666</v>
@@ -1551,19 +1542,19 @@
         <v>43859</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F17" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I17" s="1">
         <v>4.1666666666666664E-2</v>
@@ -1580,13 +1571,13 @@
         <v>43861</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1">
         <v>0.125</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>25</v>
+        <v>163</v>
       </c>
       <c r="F19" s="6">
         <v>0.125</v>
@@ -1613,24 +1604,24 @@
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>43865</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C23" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F23" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="I23" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1641,19 +1632,19 @@
         <v>43866</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="C24" s="1">
         <v>0.125</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F24" s="6">
         <v>0.125</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>38</v>
+        <v>164</v>
       </c>
       <c r="I24" s="1">
         <v>0.125</v>
@@ -1670,19 +1661,19 @@
         <v>43868</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="C26" s="1">
         <v>0.2638888888888889</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F26" s="6">
         <v>0.27083333333333331</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I26" s="1">
         <v>0.25</v>
@@ -1711,19 +1702,19 @@
         <v>43872</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C30" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="F30" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I30" s="1">
         <v>0.16666666666666666</v>
@@ -1734,19 +1725,19 @@
         <v>43873</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C31" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F31" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I31" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1763,19 +1754,19 @@
         <v>43875</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="C33" s="1">
         <v>0.25</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="F33" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I33" s="1">
         <v>0.25</v>
@@ -1811,7 +1802,7 @@
       </c>
       <c r="B38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="F38" s="6">
         <v>0.125</v>
@@ -1860,7 +1851,7 @@
       <c r="B45" s="5"/>
       <c r="C45" s="1"/>
       <c r="E45" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F45" s="6">
         <v>8.3333333333333329E-2</v>
@@ -1872,7 +1863,7 @@
         <v>43888</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C46" s="1">
         <v>6.25E-2</v>
@@ -1907,19 +1898,19 @@
         <v>43893</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="C51" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F51" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I51" s="1">
         <v>8.3333333333333329E-2</v>
@@ -1930,19 +1921,19 @@
         <v>43894</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="C52" s="1">
         <v>0.125</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F52" s="6">
         <v>0.125</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I52" s="1">
         <v>0.125</v>
@@ -1959,19 +1950,19 @@
         <v>43896</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="C54" s="1">
         <v>0.25</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F54" s="6">
         <v>0.25</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="I54" s="1">
         <v>0.25</v>
@@ -2000,19 +1991,19 @@
         <v>43900</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C58" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F58" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="I58" s="1">
         <v>0.16666666666666666</v>
@@ -2023,19 +2014,19 @@
         <v>43901</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C59" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F59" s="6">
         <v>0.125</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>53</v>
+        <v>165</v>
       </c>
       <c r="I59" s="1">
         <v>8.3333333333333329E-2</v>
@@ -2052,19 +2043,19 @@
         <v>43903</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="C61" s="1">
         <v>0.25</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="F61" s="6">
         <v>0.25</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>50</v>
+        <v>166</v>
       </c>
       <c r="I61" s="1">
         <v>0.25</v>
@@ -2088,13 +2079,13 @@
       </c>
       <c r="B64" s="5"/>
       <c r="E64" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F64" s="6">
         <v>0.14583333333333334</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>52</v>
+        <v>167</v>
       </c>
       <c r="I64" s="1">
         <v>0.16666666666666666</v>
@@ -2105,19 +2096,19 @@
         <v>43907</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="C65" s="1">
         <v>0.125</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F65" s="6">
         <v>0.1875</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I65" s="1">
         <v>0.20833333333333334</v>
@@ -2128,19 +2119,19 @@
         <v>43908</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C66" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F66" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>58</v>
+        <v>168</v>
       </c>
       <c r="I66" s="1">
         <v>8.3333333333333329E-2</v>
@@ -2152,13 +2143,13 @@
       </c>
       <c r="B67" s="5"/>
       <c r="E67" s="5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F67" s="6">
         <v>0.125</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>59</v>
+        <v>169</v>
       </c>
       <c r="I67" s="1">
         <v>0.16666666666666666</v>
@@ -2169,13 +2160,13 @@
         <v>43910</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="C68" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F68" s="6">
         <v>0.16666666666666666</v>
@@ -2198,19 +2189,19 @@
         <v>43913</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C71" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F71" s="6">
         <v>0.125</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="I71" s="1">
         <v>6.25E-2</v>
@@ -2221,19 +2212,19 @@
         <v>43914</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C72" s="1">
         <v>0.125</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>179</v>
+        <v>150</v>
       </c>
       <c r="F72" s="6">
         <v>0.125</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="I72" s="1">
         <v>0.20833333333333334</v>
@@ -2245,13 +2236,13 @@
       </c>
       <c r="B73" s="5"/>
       <c r="E73" s="5" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F73" s="6">
         <v>0.20833333333333334</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="I73" s="1">
         <v>8.3333333333333329E-2</v>
@@ -2262,19 +2253,19 @@
         <v>43916</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="C74" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F74" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="I74" s="1">
         <v>0.20833333333333334</v>
@@ -2285,19 +2276,19 @@
         <v>43917</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C75" s="1">
         <v>0.125</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>180</v>
+        <v>151</v>
       </c>
       <c r="F75" s="6">
         <v>0.1875</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="I75" s="1">
         <v>0.125</v>
@@ -2320,19 +2311,19 @@
         <v>43920</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="C78" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F78" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="I78" s="1">
         <v>8.3333333333333329E-2</v>
@@ -2343,19 +2334,19 @@
         <v>43921</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="C79" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>181</v>
+        <v>152</v>
       </c>
       <c r="F79" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2364,13 +2355,13 @@
       </c>
       <c r="B80" s="5"/>
       <c r="E80" s="5" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F80" s="6">
         <v>0.10416666666666667</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="I80" s="1">
         <v>0.125</v>
@@ -2388,19 +2379,19 @@
         <v>43924</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="C82" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F82" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>78</v>
+        <v>170</v>
       </c>
       <c r="I82" s="1">
         <v>0.125</v>
@@ -2424,19 +2415,19 @@
         <v>43927</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="C85" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="F85" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>79</v>
+        <v>171</v>
       </c>
       <c r="I85" s="1">
         <v>0.16666666666666666</v>
@@ -2447,19 +2438,19 @@
         <v>43928</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C86" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="F86" s="6">
         <v>0.125</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>84</v>
+        <v>172</v>
       </c>
       <c r="I86" s="1">
         <v>0.16666666666666666</v>
@@ -2470,19 +2461,19 @@
         <v>43929</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="C87" s="1">
         <v>0.125</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="F87" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
       <c r="I87" s="1">
         <v>0.125</v>
@@ -2493,19 +2484,19 @@
         <v>43930</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="C88" s="1">
         <v>0.125</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="F88" s="6">
         <v>0.10416666666666667</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="I88" s="1">
         <v>0.20833333333333334</v>
@@ -2516,19 +2507,19 @@
         <v>43931</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="C89" s="1">
         <v>0.125</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="F89" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H89" s="17" t="s">
-        <v>113</v>
+        <v>175</v>
       </c>
       <c r="I89" s="1">
         <v>0.125</v>
@@ -2551,15 +2542,16 @@
         <v>43934</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="C92" s="1">
         <v>0.20833333333333334</v>
       </c>
-      <c r="E92" s="18"/>
-      <c r="F92" s="19"/>
+      <c r="D92" s="25"/>
+      <c r="E92" s="26"/>
+      <c r="F92" s="27"/>
       <c r="H92" s="5" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
       <c r="I92" s="1">
         <v>0.20833333333333334</v>
@@ -2570,13 +2562,13 @@
         <v>43935</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="C93" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>90</v>
+        <v>153</v>
       </c>
       <c r="F93" s="6">
         <v>0.16666666666666666</v>
@@ -2587,13 +2579,13 @@
         <v>43936</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="C94" s="1">
         <v>0.20833333333333334</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="F94" s="6">
         <v>0.16666666666666666</v>
@@ -2605,13 +2597,13 @@
       </c>
       <c r="B95" s="5"/>
       <c r="E95" s="5" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="F95" s="6">
         <v>0.1875</v>
       </c>
       <c r="H95" s="17" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="I95" s="1">
         <v>0.125</v>
@@ -2623,13 +2615,13 @@
       </c>
       <c r="B96" s="5"/>
       <c r="E96" s="5" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F96" s="6">
         <v>0.1875</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="I96" s="1">
         <v>0.20833333333333334</v>
@@ -2652,19 +2644,19 @@
         <v>43941</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="C99" s="1">
         <v>0.125</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="F99" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H99" s="17" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="I99" s="1">
         <v>0.125</v>
@@ -2675,19 +2667,19 @@
         <v>43942</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C100" s="1">
         <v>0.125</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="F100" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H100" s="17" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="I100" s="1">
         <v>0.125</v>
@@ -2698,19 +2690,19 @@
         <v>43943</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C101" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="F101" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="I101" s="1">
         <v>0.125</v>
@@ -2721,19 +2713,19 @@
         <v>43944</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="C102" s="1">
         <v>0.14583333333333334</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="F102" s="6">
         <v>0.10416666666666667</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="I102" s="1">
         <v>0.20833333333333334</v>
@@ -2744,19 +2736,19 @@
         <v>43945</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C103" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="F103" s="6">
         <v>0.10416666666666667</v>
       </c>
       <c r="H103" s="5" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="I103" s="1">
         <v>0.20833333333333334</v>
@@ -2779,19 +2771,19 @@
         <v>43948</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C106" s="1">
         <v>0.20833333333333334</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F106" s="6">
         <v>0.1875</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>108</v>
+        <v>178</v>
       </c>
       <c r="I106" s="1">
         <v>0.20833333333333334</v>
@@ -2802,19 +2794,19 @@
         <v>43949</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C107" s="1">
         <v>0.25</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>102</v>
+        <v>154</v>
       </c>
       <c r="F107" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>109</v>
+        <v>179</v>
       </c>
       <c r="I107" s="1">
         <v>0.20833333333333334</v>
@@ -2825,19 +2817,19 @@
         <v>43950</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="C108" s="1">
         <v>0.39583333333333331</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="F108" s="6">
         <v>0.1875</v>
       </c>
       <c r="H108" s="5" t="s">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="I108" s="1">
         <v>0.125</v>
@@ -2848,19 +2840,19 @@
         <v>43951</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C109" s="1">
         <v>0.125</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="F109" s="6">
         <v>0.25</v>
       </c>
       <c r="H109" s="17" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="I109" s="1">
         <v>0.20833333333333334</v>
@@ -2871,19 +2863,19 @@
         <v>43952</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C110" s="1">
         <v>0.20833333333333334</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="F110" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H110" s="17" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="I110" s="1">
         <v>0.20833333333333334</v>
@@ -2894,19 +2886,19 @@
         <v>43953</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="C111" s="1">
         <v>0.25</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="F111" s="6">
         <v>0.10416666666666667</v>
       </c>
       <c r="H111" s="17" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="I111" s="1">
         <v>0.125</v>
@@ -2917,13 +2909,13 @@
         <v>43954</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="C112" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="H112" s="17" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="I112" s="1">
         <v>8.3333333333333329E-2</v>
@@ -2934,19 +2926,19 @@
         <v>43955</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="C113" s="1">
         <v>0.1875</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="F113" s="6">
         <v>0.1875</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>123</v>
+        <v>181</v>
       </c>
       <c r="I113" s="1">
         <v>0.20833333333333334</v>
@@ -2957,19 +2949,19 @@
         <v>43956</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="C114" s="1">
         <v>0.15277777777777776</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="F114" s="6">
-        <v>0.10416666666666667</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>124</v>
+        <v>182</v>
       </c>
       <c r="I114" s="1">
         <v>0.16666666666666666</v>
@@ -2981,13 +2973,13 @@
       </c>
       <c r="B115" s="5"/>
       <c r="E115" s="5" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="F115" s="6">
         <v>0.125</v>
       </c>
       <c r="H115" s="5" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="I115" s="1">
         <v>0.16666666666666666</v>
@@ -2998,19 +2990,19 @@
         <v>43958</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="C116" s="1">
         <v>0.125</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="F116" s="6">
         <v>0.14583333333333334</v>
       </c>
       <c r="H116" s="5" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="I116" s="1">
         <v>0.20833333333333334</v>
@@ -3021,7 +3013,7 @@
         <v>43959</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="C117" s="1">
         <v>0.20833333333333334</v>
@@ -3044,19 +3036,19 @@
         <v>43962</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C120" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="F120" s="6">
         <v>0.125</v>
       </c>
       <c r="H120" s="17" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="I120" s="1">
         <v>0.125</v>
@@ -3067,19 +3059,19 @@
         <v>43963</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="C121" s="1">
         <v>0.20833333333333334</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="F121" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="H121" s="17" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="I121" s="1">
         <v>0.125</v>
@@ -3090,19 +3082,19 @@
         <v>43964</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="C122" s="1">
         <v>0.20833333333333334</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="F122" s="6">
         <v>0.22916666666666666</v>
       </c>
       <c r="H122" s="17" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="I122" s="1">
         <v>0.20833333333333334</v>
@@ -3113,13 +3105,13 @@
         <v>43965</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C123" s="1">
         <v>0.1875</v>
       </c>
       <c r="H123" s="17" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="I123" s="1">
         <v>0.1875</v>
@@ -3130,19 +3122,19 @@
         <v>43966</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C124" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="F124" s="6">
         <v>0.27083333333333331</v>
       </c>
       <c r="H124" s="17" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="I124" s="1">
         <v>0.16666666666666666</v>
@@ -3153,7 +3145,7 @@
         <v>43967</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C125" s="1">
         <v>0.20833333333333334</v>
@@ -3164,7 +3156,7 @@
         <v>43968</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C126" s="1">
         <v>0.25</v>
@@ -3175,19 +3167,19 @@
         <v>43969</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C127" s="1">
         <v>0.16666666666666666</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="F127" s="6">
         <v>0.14583333333333334</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="I127" s="1">
         <v>0.125</v>
@@ -3198,13 +3190,13 @@
         <v>43970</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C128" s="1">
         <v>0.125</v>
       </c>
       <c r="H128" s="17" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="I128" s="1">
         <v>8.3333333333333329E-2</v>
@@ -3245,7 +3237,7 @@
         <v>43976</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="C134" s="1">
         <v>0.16666666666666666</v>
@@ -3256,7 +3248,7 @@
         <v>43977</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="C135" s="1">
         <v>0.16666666666666666</v>
@@ -3267,7 +3259,7 @@
         <v>43978</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="C136" s="1">
         <v>0.20833333333333334</v>
@@ -3278,13 +3270,13 @@
         <v>43979</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="C137" s="1">
         <v>0.125</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="F137" s="6">
         <v>8.3333333333333329E-2</v>
@@ -3295,13 +3287,13 @@
         <v>43980</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="C138" s="1">
         <v>0.29166666666666669</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="F138" s="6">
         <v>0.125</v>
@@ -3324,7 +3316,7 @@
         <v>43983</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="C141" s="1">
         <v>0.33333333333333331</v>
@@ -3335,13 +3327,13 @@
         <v>43984</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="C142" s="1">
         <v>0.29166666666666669</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="F142" s="6">
         <v>0.14583333333333334</v>
@@ -3353,7 +3345,7 @@
       </c>
       <c r="B143" s="5"/>
       <c r="E143" s="5" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="F143" s="6">
         <v>0.16666666666666666</v>
@@ -3393,23 +3385,23 @@
       <c r="A149" s="3">
         <v>43991</v>
       </c>
-      <c r="B149" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="C149" s="20">
+      <c r="B149" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C149" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D149" s="22"/>
-      <c r="E149" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="F149" s="21">
+      <c r="D149" s="20"/>
+      <c r="E149" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F149" s="19">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="H149" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="I149" s="20">
+      <c r="H149" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="I149" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -3453,15 +3445,15 @@
       <c r="A159" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C159" s="25">
+      <c r="C159" s="23">
         <f>SUM(C2:C155)</f>
         <v>11.260416666666664</v>
       </c>
-      <c r="F159" s="25">
+      <c r="F159" s="23">
         <f>SUM(F2:F155)</f>
-        <v>10.375000000000002</v>
-      </c>
-      <c r="I159" s="26">
+        <v>10.41666666666667</v>
+      </c>
+      <c r="I159" s="24">
         <f>SUM(I2:I155)</f>
         <v>9.6666666666666643</v>
       </c>

</xml_diff>

<commit_message>
Mise à jour du journal d'activités (de ce week-end).
</commit_message>
<xml_diff>
--- a/Commun/Journal d'activités.xlsx
+++ b/Commun/Journal d'activités.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Guillaume\BTS SN\Projet Systeme-Escape-Game-Telethon\Systeme-Escape-Game-Telethon\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Systeme-Escape-Game-Telethon\Commun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B210D313-1CA7-4F4E-A85F-B1669E3FC3A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C7134F-F883-4A53-B75A-5888C545873B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4456A671-B883-4442-B94A-6163F7130CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="198">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -718,6 +718,12 @@
   </si>
   <si>
     <t>Préparation revue final</t>
+  </si>
+  <si>
+    <t>Entrainement au passage de la revue finale.</t>
+  </si>
+  <si>
+    <t>Finalisation du diaporama (chemin de fer, mise en forme, mise à jour de certains élements…). Entrainements à la présentation, tests du fonctionnement du matériel avec le suivi des fiches recettes. Préparation de la présentation matérielle.</t>
   </si>
 </sst>
 </file>
@@ -1339,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E36E91A-450F-447C-A131-782583851794}">
   <dimension ref="A1:J154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L132" sqref="L132"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3481,6 +3487,12 @@
       <c r="C146" s="1">
         <v>0.20833333333333334</v>
       </c>
+      <c r="E146" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F146" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
@@ -3488,11 +3500,17 @@
       </c>
       <c r="B147" s="5"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>43990</v>
       </c>
       <c r="B148" s="5"/>
+      <c r="E148" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F148" s="6">
+        <v>0.20833333333333334</v>
+      </c>
     </row>
     <row r="149" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
@@ -3528,7 +3546,7 @@
       </c>
       <c r="F153" s="23">
         <f>SUM(F2:F149)</f>
-        <v>10.770833333333336</v>
+        <v>11.020833333333336</v>
       </c>
       <c r="I153" s="24">
         <f>SUM(I2:I149)</f>

</xml_diff>